<commit_message>
edited combined attributes dataset
</commit_message>
<xml_diff>
--- a/Data/Combined Attributes.xlsx
+++ b/Data/Combined Attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yi Zhen\Documents\GitHub\BT4015\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2CA7F1-256C-4DCB-97DF-FE24DA743A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB53B45E-B221-4C91-A445-68B920B0FA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
     <col min="9" max="11" width="9.36328125" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -624,48 +624,48 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9">
-        <f>SUM(B3:B32)</f>
+        <f t="shared" ref="B2:K2" si="0">SUM(B3:B32)</f>
         <v>4010200</v>
       </c>
       <c r="C2" s="8">
-        <f>SUM(C3:C32)</f>
+        <f t="shared" si="0"/>
         <v>516681</v>
       </c>
       <c r="D2" s="8">
-        <f>SUM(D3:D32)</f>
+        <f t="shared" si="0"/>
         <v>662911</v>
       </c>
       <c r="E2" s="9">
-        <f>SUM(E3:E32)</f>
+        <f t="shared" si="0"/>
         <v>1075957</v>
       </c>
       <c r="F2" s="9">
-        <f>SUM(F3:F32)</f>
+        <f t="shared" si="0"/>
         <v>1179592</v>
       </c>
       <c r="G2" s="9">
-        <f>SUM(G3:G32)</f>
+        <f t="shared" si="0"/>
         <v>891370</v>
       </c>
       <c r="H2" s="11">
-        <f>SUM(H3:H32)</f>
+        <f t="shared" si="0"/>
         <v>2982590</v>
       </c>
       <c r="I2" s="11">
-        <f>SUM(I3:I32)</f>
+        <f t="shared" si="0"/>
         <v>544020</v>
       </c>
       <c r="J2" s="11">
-        <f>SUM(J3:J32)</f>
+        <f t="shared" si="0"/>
         <v>357670</v>
       </c>
       <c r="K2" s="11">
-        <f>SUM(K3:K32)</f>
+        <f t="shared" si="0"/>
         <v>125910</v>
       </c>
       <c r="L2" s="9">
@@ -676,12 +676,8 @@
         <f>SUM(M3:M32)</f>
         <v>2049270</v>
       </c>
-      <c r="N2" s="9">
-        <f>L2+M2</f>
-        <v>3932680</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -698,7 +694,7 @@
         <v>50647</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F32" si="0">C3+D3</f>
+        <f t="shared" ref="F3:F32" si="1">C3+D3</f>
         <v>48763</v>
       </c>
       <c r="G3">
@@ -722,12 +718,8 @@
       <c r="M3">
         <v>84700</v>
       </c>
-      <c r="N3">
-        <f>H2+I2+J2+K2</f>
-        <v>4010190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -744,7 +736,7 @@
         <v>64565</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80735</v>
       </c>
       <c r="G4">
@@ -769,7 +761,7 @@
         <v>142790</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -786,7 +778,7 @@
         <v>20547</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25032</v>
       </c>
       <c r="G5">
@@ -811,7 +803,7 @@
         <v>45060</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -828,7 +820,7 @@
         <v>43387</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48315</v>
       </c>
       <c r="G6">
@@ -853,7 +845,7 @@
         <v>80550</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -870,7 +862,7 @@
         <v>53875</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47257</v>
       </c>
       <c r="G7">
@@ -895,7 +887,7 @@
         <v>78520</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -912,7 +904,7 @@
         <v>36120</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39190</v>
       </c>
       <c r="G8">
@@ -937,7 +929,7 @@
         <v>70120</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -954,7 +946,7 @@
         <v>2493</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20766</v>
       </c>
       <c r="G9">
@@ -979,7 +971,7 @@
         <v>41880</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -996,7 +988,7 @@
         <v>50018</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53561</v>
       </c>
       <c r="G10">
@@ -1021,7 +1013,7 @@
         <v>96380</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1038,7 +1030,7 @@
         <v>25820</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27619</v>
       </c>
       <c r="G11">
@@ -1063,7 +1055,7 @@
         <v>48360</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1080,7 +1072,7 @@
         <v>229</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1371</v>
       </c>
       <c r="G12">
@@ -1105,7 +1097,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1114,7 @@
         <v>30971</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35070</v>
       </c>
       <c r="G13">
@@ -1147,7 +1139,7 @@
         <v>55860</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1164,7 +1156,7 @@
         <v>57979</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66608</v>
       </c>
       <c r="G14">
@@ -1189,7 +1181,7 @@
         <v>116070</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1206,7 +1198,7 @@
         <v>24649</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22958</v>
       </c>
       <c r="G15">
@@ -1231,7 +1223,7 @@
         <v>39670</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1248,7 +1240,7 @@
         <v>77166</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>75808</v>
       </c>
       <c r="G16">
@@ -1290,7 +1282,7 @@
         <v>32257</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32401</v>
       </c>
       <c r="G17">
@@ -1332,7 +1324,7 @@
         <v>7993</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13518</v>
       </c>
       <c r="G18">
@@ -1374,7 +1366,7 @@
         <v>8370</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15435</v>
       </c>
       <c r="G19">
@@ -1416,7 +1408,7 @@
         <v>7605</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5859</v>
       </c>
       <c r="G20">
@@ -1458,7 +1450,7 @@
         <v>30080</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41097</v>
       </c>
       <c r="G21">
@@ -1500,7 +1492,7 @@
         <v>49035</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52635</v>
       </c>
       <c r="G22">
@@ -1542,7 +1534,7 @@
         <v>31259</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29278</v>
       </c>
       <c r="G23">
@@ -1584,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3403</v>
       </c>
       <c r="G24">
@@ -1626,7 +1618,7 @@
         <v>28584</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30335</v>
       </c>
       <c r="G25">
@@ -1668,7 +1660,7 @@
         <v>68180</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73754</v>
       </c>
       <c r="G26">
@@ -1710,7 +1702,7 @@
         <v>22085</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32768</v>
       </c>
       <c r="G27">
@@ -1752,7 +1744,7 @@
         <v>72846</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>74051</v>
       </c>
       <c r="G28">
@@ -1794,7 +1786,7 @@
         <v>187</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6727</v>
       </c>
       <c r="G29">
@@ -1836,7 +1828,7 @@
         <v>39272</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36865</v>
       </c>
       <c r="G30">
@@ -1878,7 +1870,7 @@
         <v>72965</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71709</v>
       </c>
       <c r="G31">
@@ -1920,7 +1912,7 @@
         <v>66773</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66704</v>
       </c>
       <c r="G32">

</xml_diff>

<commit_message>
Cleaned Land Area and appended to combined attributes file, Calculate some ratios in combined attributes file
</commit_message>
<xml_diff>
--- a/Data/Combined Attributes.xlsx
+++ b/Data/Combined Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yi Zhen\Documents\GitHub\BT4015\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0DE555-FED6-4053-B8F7-86507EFEFC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC98B23-209E-41CD-B8A3-9E15E153D28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="830" yWindow="230" windowWidth="18320" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Planning Area of Residence</t>
   </si>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t xml:space="preserve">Households Above Median Income </t>
+  </si>
+  <si>
+    <t>Area of Planning Area</t>
+  </si>
+  <si>
+    <t>Elderly Ratio</t>
+  </si>
+  <si>
+    <t>Chinese Ratio</t>
+  </si>
+  <si>
+    <t>Malay Ratio</t>
+  </si>
+  <si>
+    <t>Indian Ratio</t>
+  </si>
+  <si>
+    <t>Others Ratio</t>
   </si>
 </sst>
 </file>
@@ -256,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -284,6 +302,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,1377 +586,2110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" style="3" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.36328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="9.36328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.90625" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9">
-        <f t="shared" ref="B2:K2" si="0">SUM(B3:B32)</f>
+        <f t="shared" ref="B2:L2" si="0">SUM(B3:B32)</f>
         <v>4010200</v>
       </c>
-      <c r="C2" s="8">
+      <c r="D2" s="8">
         <f t="shared" si="0"/>
         <v>516681</v>
       </c>
-      <c r="D2" s="8">
+      <c r="E2" s="8">
         <f t="shared" si="0"/>
         <v>662911</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F2" s="9">
         <f t="shared" si="0"/>
         <v>1075957</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="9">
         <f t="shared" si="0"/>
         <v>1179592</v>
       </c>
-      <c r="G2" s="9">
+      <c r="H2" s="9">
         <f t="shared" si="0"/>
         <v>891370</v>
       </c>
-      <c r="H2" s="11">
+      <c r="I2" s="11">
         <f t="shared" si="0"/>
         <v>2982590</v>
       </c>
-      <c r="I2" s="11">
+      <c r="J2" s="11">
         <f t="shared" si="0"/>
         <v>544020</v>
       </c>
-      <c r="J2" s="11">
+      <c r="K2" s="11">
         <f t="shared" si="0"/>
         <v>357670</v>
       </c>
-      <c r="K2" s="11">
+      <c r="L2" s="11">
         <f t="shared" si="0"/>
         <v>125910</v>
       </c>
-      <c r="L2" s="9">
-        <f>SUM(L4:L32)</f>
+      <c r="M2" s="9">
+        <f>SUM(M4:M32)</f>
         <v>1883410</v>
       </c>
-      <c r="M2" s="9">
-        <f>SUM(M3:M32)</f>
+      <c r="N2" s="9">
+        <f>SUM(N3:N32)</f>
         <v>2049270</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O2" s="9">
+        <f>H2/B2</f>
+        <v>0.22227569697271957</v>
+      </c>
+      <c r="P2" s="9">
+        <f>I2/B2</f>
+        <v>0.74375093511545554</v>
+      </c>
+      <c r="Q2" s="9">
+        <f>M2/B2</f>
+        <v>0.46965488005585754</v>
+      </c>
+      <c r="R2" s="9">
+        <f>K2/B2</f>
+        <v>8.9190065333399834E-2</v>
+      </c>
+      <c r="S2" s="9">
+        <f>L2/B2</f>
+        <v>3.139743653683108E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>162280</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
+        <v>13942583.369999999</v>
+      </c>
+      <c r="D3" s="2">
         <v>25513</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>23250</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>50647</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F32" si="1">C3+D3</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G32" si="1">D3+E3</f>
         <v>48763</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>47950</v>
       </c>
-      <c r="H3" s="10">
+      <c r="I3" s="10">
         <v>134350</v>
       </c>
-      <c r="I3" s="10">
+      <c r="J3" s="10">
         <v>11140</v>
       </c>
-      <c r="J3" s="10">
+      <c r="K3" s="10">
         <v>12810</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="10">
         <v>3970</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>77570</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>84700</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O3" s="16">
+        <f t="shared" ref="O3:O32" si="2">H3/B3</f>
+        <v>0.29547695341385261</v>
+      </c>
+      <c r="P3" s="16">
+        <f t="shared" ref="P3:P32" si="3">I3/B3</f>
+        <v>0.8278900665516391</v>
+      </c>
+      <c r="Q3" s="16">
+        <f t="shared" ref="Q3:Q32" si="4">M3/B3</f>
+        <v>0.47800098595020951</v>
+      </c>
+      <c r="R3" s="16">
+        <f t="shared" ref="R3:R32" si="5">K3/B3</f>
+        <v>7.8937638649248215E-2</v>
+      </c>
+      <c r="S3" s="16">
+        <f t="shared" ref="S3:S32" si="6">L3/B3</f>
+        <v>2.4463889573576536E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>276990</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
+        <v>48665179.850000001</v>
+      </c>
+      <c r="D4" s="2">
         <v>36087</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>44648</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>64565</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="1"/>
         <v>80735</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>75230</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="10">
         <v>201780</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="10">
         <v>39300</v>
       </c>
-      <c r="J4" s="10">
+      <c r="K4" s="10">
         <v>24450</v>
       </c>
-      <c r="K4" s="10">
+      <c r="L4" s="10">
         <v>11470</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>134210</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>142790</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O4" s="16">
+        <f t="shared" si="2"/>
+        <v>0.27159825264449983</v>
+      </c>
+      <c r="P4" s="16">
+        <f t="shared" si="3"/>
+        <v>0.72847395212823562</v>
+      </c>
+      <c r="Q4" s="16">
+        <f t="shared" si="4"/>
+        <v>0.48453012744142387</v>
+      </c>
+      <c r="R4" s="16">
+        <f t="shared" si="5"/>
+        <v>8.8270334669121625E-2</v>
+      </c>
+      <c r="S4" s="16">
+        <f t="shared" si="6"/>
+        <v>4.1409437163796525E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>87320</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
+        <v>7608112.5300000003</v>
+      </c>
+      <c r="D5" s="2">
         <v>8259</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>16773</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>20547</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>25032</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>23170</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="10">
         <v>75040</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="10">
         <v>3190</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <v>6490</v>
       </c>
-      <c r="K5" s="10">
+      <c r="L5" s="10">
         <v>2590</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>42260</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>45060</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O5" s="16">
+        <f t="shared" si="2"/>
+        <v>0.26534585432890517</v>
+      </c>
+      <c r="P5" s="16">
+        <f t="shared" si="3"/>
+        <v>0.85936784241868991</v>
+      </c>
+      <c r="Q5" s="16">
+        <f t="shared" si="4"/>
+        <v>0.48396701786532292</v>
+      </c>
+      <c r="R5" s="16">
+        <f t="shared" si="5"/>
+        <v>7.4324324324324328E-2</v>
+      </c>
+      <c r="S5" s="16">
+        <f t="shared" si="6"/>
+        <v>2.9661016949152543E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>158030</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
+        <v>11140156.279999999</v>
+      </c>
+      <c r="D6" s="2">
         <v>22192</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>26123</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>43387</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>48315</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>33420</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="10">
         <v>113460</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="10">
         <v>25240</v>
       </c>
-      <c r="J6" s="10">
+      <c r="K6" s="10">
         <v>14950</v>
       </c>
-      <c r="K6" s="10">
+      <c r="L6" s="10">
         <v>4380</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>77480</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>80550</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O6" s="16">
+        <f t="shared" si="2"/>
+        <v>0.21147883313294943</v>
+      </c>
+      <c r="P6" s="16">
+        <f t="shared" si="3"/>
+        <v>0.71796494336518379</v>
+      </c>
+      <c r="Q6" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49028665443270264</v>
+      </c>
+      <c r="R6" s="16">
+        <f t="shared" si="5"/>
+        <v>9.4602290704296654E-2</v>
+      </c>
+      <c r="S6" s="16">
+        <f t="shared" si="6"/>
+        <v>2.7716256407011326E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>151250</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
+        <v>17774660.609999999</v>
+      </c>
+      <c r="D7" s="2">
         <v>22749</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="2">
         <v>24508</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>53875</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>47257</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>44420</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="10">
         <v>120830</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="10">
         <v>11430</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="10">
         <v>13980</v>
       </c>
-      <c r="K7" s="10">
+      <c r="L7" s="10">
         <v>5010</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>72730</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>78520</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O7" s="16">
+        <f t="shared" si="2"/>
+        <v>0.29368595041322315</v>
+      </c>
+      <c r="P7" s="16">
+        <f t="shared" si="3"/>
+        <v>0.79887603305785126</v>
+      </c>
+      <c r="Q7" s="16">
+        <f t="shared" si="4"/>
+        <v>0.48085950413223139</v>
+      </c>
+      <c r="R7" s="16">
+        <f t="shared" si="5"/>
+        <v>9.24297520661157E-2</v>
+      </c>
+      <c r="S7" s="16">
+        <f t="shared" si="6"/>
+        <v>3.312396694214876E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>138270</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
+        <v>9019929.7300000004</v>
+      </c>
+      <c r="D8" s="2">
         <v>17434</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>21756</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>36120</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>39190</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>27890</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="10">
         <v>102800</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="10">
         <v>21690</v>
       </c>
-      <c r="J8" s="10">
+      <c r="K8" s="10">
         <v>10340</v>
       </c>
-      <c r="K8" s="10">
+      <c r="L8" s="10">
         <v>3450</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>68150</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>70120</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O8" s="16">
+        <f t="shared" si="2"/>
+        <v>0.20170680552542128</v>
+      </c>
+      <c r="P8" s="16">
+        <f t="shared" si="3"/>
+        <v>0.74347291531062409</v>
+      </c>
+      <c r="Q8" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49287625659940698</v>
+      </c>
+      <c r="R8" s="16">
+        <f t="shared" si="5"/>
+        <v>7.4781225139220364E-2</v>
+      </c>
+      <c r="S8" s="16">
+        <f t="shared" si="6"/>
+        <v>2.495118246908223E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
         <v>77860</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
+        <v>17514936.539999999</v>
+      </c>
+      <c r="D9" s="2">
         <v>3610</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>17156</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2493</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="1"/>
         <v>20766</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>18040</v>
       </c>
-      <c r="H9" s="10">
+      <c r="I9" s="10">
         <v>67400</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="10">
         <v>640</v>
       </c>
-      <c r="J9" s="10">
+      <c r="K9" s="10">
         <v>3840</v>
       </c>
-      <c r="K9" s="10">
+      <c r="L9" s="10">
         <v>5980</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>35980</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>41880</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O9" s="16">
+        <f t="shared" si="2"/>
+        <v>0.23169791934240946</v>
+      </c>
+      <c r="P9" s="16">
+        <f t="shared" si="3"/>
+        <v>0.86565630619059852</v>
+      </c>
+      <c r="Q9" s="16">
+        <f t="shared" si="4"/>
+        <v>0.46211148214744413</v>
+      </c>
+      <c r="R9" s="16">
+        <f t="shared" si="5"/>
+        <v>4.9319291035191372E-2</v>
+      </c>
+      <c r="S9" s="16">
+        <f t="shared" si="6"/>
+        <v>7.6804520935011555E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>192070</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
+        <v>6117280.0489999996</v>
+      </c>
+      <c r="D10" s="2">
         <v>21847</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>31714</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>50018</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="1"/>
         <v>53561</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>32830</v>
       </c>
-      <c r="H10" s="10">
+      <c r="I10" s="10">
         <v>133520</v>
       </c>
-      <c r="I10" s="10">
+      <c r="J10" s="10">
         <v>35500</v>
       </c>
-      <c r="J10" s="10">
+      <c r="K10" s="10">
         <v>18020</v>
       </c>
-      <c r="K10" s="10">
+      <c r="L10" s="10">
         <v>5020</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>95690</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>96380</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O10" s="16">
+        <f t="shared" si="2"/>
+        <v>0.17092726610090073</v>
+      </c>
+      <c r="P10" s="16">
+        <f t="shared" si="3"/>
+        <v>0.69516322174207323</v>
+      </c>
+      <c r="Q10" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49820377987192171</v>
+      </c>
+      <c r="R10" s="16">
+        <f t="shared" si="5"/>
+        <v>9.3819961472379865E-2</v>
+      </c>
+      <c r="S10" s="16">
+        <f t="shared" si="6"/>
+        <v>2.6136304472327797E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11">
         <v>91990</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
+        <v>9524177.7479999997</v>
+      </c>
+      <c r="D11" s="2">
         <v>11433</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="2">
         <v>16186</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>25820</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="1"/>
         <v>27619</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>24700</v>
       </c>
-      <c r="H11" s="10">
+      <c r="I11" s="10">
         <v>73630</v>
       </c>
-      <c r="I11" s="10">
+      <c r="J11" s="10">
         <v>8270</v>
       </c>
-      <c r="J11" s="10">
+      <c r="K11" s="10">
         <v>6970</v>
       </c>
-      <c r="K11" s="10">
+      <c r="L11" s="10">
         <v>3120</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>43630</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>48360</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O11" s="16">
+        <f t="shared" si="2"/>
+        <v>0.26850744646157193</v>
+      </c>
+      <c r="P11" s="16">
+        <f t="shared" si="3"/>
+        <v>0.80041308837917169</v>
+      </c>
+      <c r="Q11" s="16">
+        <f t="shared" si="4"/>
+        <v>0.47429068376997502</v>
+      </c>
+      <c r="R11" s="16">
+        <f t="shared" si="5"/>
+        <v>7.5769105337536682E-2</v>
+      </c>
+      <c r="S11" s="16">
+        <f t="shared" si="6"/>
+        <v>3.3916730079356451E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12">
         <v>3190</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
+        <v>5083636.2889999999</v>
+      </c>
+      <c r="D12" s="2">
         <v>260</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>1111</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>229</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="1"/>
         <v>1371</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>630</v>
       </c>
-      <c r="H12" s="10">
+      <c r="I12" s="10">
         <v>2500</v>
       </c>
-      <c r="I12" s="10">
+      <c r="J12" s="10">
         <v>30</v>
       </c>
-      <c r="J12" s="10">
+      <c r="K12" s="10">
         <v>200</v>
       </c>
-      <c r="K12" s="10">
+      <c r="L12" s="10">
         <v>460</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1590</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>1600</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O12" s="16">
+        <f t="shared" si="2"/>
+        <v>0.19749216300940439</v>
+      </c>
+      <c r="P12" s="16">
+        <f t="shared" si="3"/>
+        <v>0.78369905956112851</v>
+      </c>
+      <c r="Q12" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49843260188087773</v>
+      </c>
+      <c r="R12" s="16">
+        <f t="shared" si="5"/>
+        <v>6.2695924764890276E-2</v>
+      </c>
+      <c r="S12" s="16">
+        <f t="shared" si="6"/>
+        <v>0.14420062695924765</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13">
         <v>110110</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
+        <v>9644787.3660000004</v>
+      </c>
+      <c r="D13" s="2">
         <v>17907</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>17163</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>30971</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>35070</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>30000</v>
       </c>
-      <c r="H13" s="10">
+      <c r="I13" s="10">
         <v>85460</v>
       </c>
-      <c r="I13" s="10">
+      <c r="J13" s="10">
         <v>12470</v>
       </c>
-      <c r="J13" s="10">
+      <c r="K13" s="10">
         <v>8640</v>
       </c>
-      <c r="K13" s="10">
+      <c r="L13" s="10">
         <v>3550</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>54260</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>55860</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O13" s="16">
+        <f t="shared" si="2"/>
+        <v>0.27245481790936338</v>
+      </c>
+      <c r="P13" s="16">
+        <f t="shared" si="3"/>
+        <v>0.77613295795113979</v>
+      </c>
+      <c r="Q13" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49277994732540187</v>
+      </c>
+      <c r="R13" s="16">
+        <f t="shared" si="5"/>
+        <v>7.8466987557896647E-2</v>
+      </c>
+      <c r="S13" s="16">
+        <f t="shared" si="6"/>
+        <v>3.2240486785941332E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <v>227560</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
+        <v>13933022.85</v>
+      </c>
+      <c r="D14" s="2">
         <v>29848</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>36760</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>57979</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <f t="shared" si="1"/>
         <v>66608</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>55530</v>
       </c>
-      <c r="H14" s="10">
+      <c r="I14" s="10">
         <v>184810</v>
       </c>
-      <c r="I14" s="10">
+      <c r="J14" s="10">
         <v>18760</v>
       </c>
-      <c r="J14" s="10">
+      <c r="K14" s="10">
         <v>18710</v>
       </c>
-      <c r="K14" s="10">
+      <c r="L14" s="10">
         <v>5290</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>111490</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>116070</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O14" s="16">
+        <f t="shared" si="2"/>
+        <v>0.2440235542274565</v>
+      </c>
+      <c r="P14" s="16">
+        <f t="shared" si="3"/>
+        <v>0.81213745825276851</v>
+      </c>
+      <c r="Q14" s="16">
+        <f t="shared" si="4"/>
+        <v>0.4899367199859378</v>
+      </c>
+      <c r="R14" s="16">
+        <f t="shared" si="5"/>
+        <v>8.2220073826683074E-2</v>
+      </c>
+      <c r="S14" s="16">
+        <f t="shared" si="6"/>
+        <v>2.3246616277025841E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15">
         <v>78600</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
+        <v>22949603.41</v>
+      </c>
+      <c r="D15" s="2">
         <v>11653</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>11305</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>24649</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>22958</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>21640</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I15" s="10">
         <v>55440</v>
       </c>
-      <c r="I15" s="10">
+      <c r="J15" s="10">
         <v>12700</v>
       </c>
-      <c r="J15" s="10">
+      <c r="K15" s="10">
         <v>8610</v>
       </c>
-      <c r="K15" s="10">
+      <c r="L15" s="10">
         <v>1850</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>38930</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>39670</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O15" s="16">
+        <f t="shared" si="2"/>
+        <v>0.27531806615776083</v>
+      </c>
+      <c r="P15" s="16">
+        <f t="shared" si="3"/>
+        <v>0.70534351145038165</v>
+      </c>
+      <c r="Q15" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49529262086513998</v>
+      </c>
+      <c r="R15" s="16">
+        <f t="shared" si="5"/>
+        <v>0.10954198473282442</v>
+      </c>
+      <c r="S15" s="16">
+        <f t="shared" si="6"/>
+        <v>2.3536895674300253E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16">
         <v>262730</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
+        <v>14680284.49</v>
+      </c>
+      <c r="D16" s="2">
         <v>35323</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>40485</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>77166</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>75808</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>51550</v>
       </c>
-      <c r="H16" s="10">
+      <c r="I16" s="10">
         <v>183590</v>
       </c>
-      <c r="I16" s="10">
+      <c r="J16" s="10">
         <v>46520</v>
       </c>
-      <c r="J16" s="10">
+      <c r="K16" s="10">
         <v>26360</v>
       </c>
-      <c r="K16" s="10">
+      <c r="L16" s="10">
         <v>6260</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>131900</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>130840</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O16" s="16">
+        <f t="shared" si="2"/>
+        <v>0.19620903589236097</v>
+      </c>
+      <c r="P16" s="16">
+        <f t="shared" si="3"/>
+        <v>0.69877821337494761</v>
+      </c>
+      <c r="Q16" s="16">
+        <f t="shared" si="4"/>
+        <v>0.50203631104175395</v>
+      </c>
+      <c r="R16" s="16">
+        <f t="shared" si="5"/>
+        <v>0.10033113843108896</v>
+      </c>
+      <c r="S16" s="16">
+        <f t="shared" si="6"/>
+        <v>2.382674228295208E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>101290</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
+        <v>8584699.8509999998</v>
+      </c>
+      <c r="D17" s="2">
         <v>15596</v>
       </c>
-      <c r="D17" s="2">
+      <c r="E17" s="2">
         <v>16805</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>32257</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>32401</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>29050</v>
       </c>
-      <c r="H17" s="10">
+      <c r="I17" s="10">
         <v>77010</v>
       </c>
-      <c r="I17" s="10">
+      <c r="J17" s="10">
         <v>7000</v>
       </c>
-      <c r="J17" s="10">
+      <c r="K17" s="10">
         <v>14510</v>
       </c>
-      <c r="K17" s="10">
+      <c r="L17" s="10">
         <v>2780</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>50040</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>51260</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O17" s="16">
+        <f t="shared" si="2"/>
+        <v>0.28680027643400136</v>
+      </c>
+      <c r="P17" s="16">
+        <f t="shared" si="3"/>
+        <v>0.76029223023003256</v>
+      </c>
+      <c r="Q17" s="16">
+        <f t="shared" si="4"/>
+        <v>0.4940270510415638</v>
+      </c>
+      <c r="R17" s="16">
+        <f t="shared" si="5"/>
+        <v>0.1432520485734031</v>
+      </c>
+      <c r="S17" s="16">
+        <f t="shared" si="6"/>
+        <v>2.7445947280086879E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>46220</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
+        <v>35044849.079999998</v>
+      </c>
+      <c r="D18" s="2">
         <v>4475</v>
       </c>
-      <c r="D18" s="2">
+      <c r="E18" s="2">
         <v>9043</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>7993</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <f t="shared" si="1"/>
         <v>13518</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>12190</v>
       </c>
-      <c r="H18" s="10">
+      <c r="I18" s="10">
         <v>35050</v>
       </c>
-      <c r="I18" s="10">
+      <c r="J18" s="10">
         <v>3120</v>
       </c>
-      <c r="J18" s="10">
+      <c r="K18" s="10">
         <v>5510</v>
       </c>
-      <c r="K18" s="10">
+      <c r="L18" s="10">
         <v>2530</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>21700</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>24520</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O18" s="16">
+        <f t="shared" si="2"/>
+        <v>0.2637386412808308</v>
+      </c>
+      <c r="P18" s="16">
+        <f t="shared" si="3"/>
+        <v>0.75832972739073989</v>
+      </c>
+      <c r="Q18" s="16">
+        <f t="shared" si="4"/>
+        <v>0.46949372565988751</v>
+      </c>
+      <c r="R18" s="16">
+        <f t="shared" si="5"/>
+        <v>0.11921246213760277</v>
+      </c>
+      <c r="S18" s="16">
+        <f t="shared" si="6"/>
+        <v>5.4738208567719604E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>49330</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
+        <v>8968011.8120000008</v>
+      </c>
+      <c r="D19" s="2">
         <v>5420</v>
       </c>
-      <c r="D19" s="2">
+      <c r="E19" s="2">
         <v>10015</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>8370</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <f t="shared" si="1"/>
         <v>15435</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>11750</v>
       </c>
-      <c r="H19" s="10">
+      <c r="I19" s="10">
         <v>40720</v>
       </c>
-      <c r="I19" s="10">
+      <c r="J19" s="10">
         <v>1730</v>
       </c>
-      <c r="J19" s="10">
+      <c r="K19" s="10">
         <v>4140</v>
       </c>
-      <c r="K19" s="10">
+      <c r="L19" s="10">
         <v>2740</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>23930</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>25400</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O19" s="16">
+        <f t="shared" si="2"/>
+        <v>0.23819176971416989</v>
+      </c>
+      <c r="P19" s="16">
+        <f t="shared" si="3"/>
+        <v>0.82546117980944655</v>
+      </c>
+      <c r="Q19" s="16">
+        <f t="shared" si="4"/>
+        <v>0.4851003446178796</v>
+      </c>
+      <c r="R19" s="16">
+        <f t="shared" si="5"/>
+        <v>8.3924589499290492E-2</v>
+      </c>
+      <c r="S19" s="16">
+        <f t="shared" si="6"/>
+        <v>5.5544293533346847E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>18340</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
+        <v>1373186.2320000001</v>
+      </c>
+      <c r="D20" s="2">
         <v>3167</v>
       </c>
-      <c r="D20" s="2">
+      <c r="E20" s="2">
         <v>2692</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>7605</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <f t="shared" si="1"/>
         <v>5859</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>6140</v>
       </c>
-      <c r="H20" s="10">
+      <c r="I20" s="10">
         <v>14910</v>
       </c>
-      <c r="I20" s="10">
+      <c r="J20" s="10">
         <v>1650</v>
       </c>
-      <c r="J20" s="10">
+      <c r="K20" s="10">
         <v>1290</v>
       </c>
-      <c r="K20" s="10">
+      <c r="L20" s="10">
         <v>480</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>9210</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>9130</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O20" s="16">
+        <f t="shared" si="2"/>
+        <v>0.33478735005452565</v>
+      </c>
+      <c r="P20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.81297709923664119</v>
+      </c>
+      <c r="Q20" s="16">
+        <f t="shared" si="4"/>
+        <v>0.50218102508178841</v>
+      </c>
+      <c r="R20" s="16">
+        <f t="shared" si="5"/>
+        <v>7.0338058887677204E-2</v>
+      </c>
+      <c r="S20" s="16">
+        <f t="shared" si="6"/>
+        <v>2.6172300981461286E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>147110</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
+        <v>20489871.34</v>
+      </c>
+      <c r="D21" s="2">
         <v>13329</v>
       </c>
-      <c r="D21" s="2">
+      <c r="E21" s="2">
         <v>27768</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>30080</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <f t="shared" si="1"/>
         <v>41097</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>26570</v>
       </c>
-      <c r="H21" s="10">
+      <c r="I21" s="10">
         <v>98790</v>
       </c>
-      <c r="I21" s="10">
+      <c r="J21" s="10">
         <v>29370</v>
       </c>
-      <c r="J21" s="10">
+      <c r="K21" s="10">
         <v>13120</v>
       </c>
-      <c r="K21" s="10">
+      <c r="L21" s="10">
         <v>5840</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>72540</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>74570</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O21" s="16">
+        <f t="shared" si="2"/>
+        <v>0.18061314662497452</v>
+      </c>
+      <c r="P21" s="16">
+        <f t="shared" si="3"/>
+        <v>0.67153830466997488</v>
+      </c>
+      <c r="Q21" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49310040106043096</v>
+      </c>
+      <c r="R21" s="16">
+        <f t="shared" si="5"/>
+        <v>8.9184963632655836E-2</v>
+      </c>
+      <c r="S21" s="16">
+        <f t="shared" si="6"/>
+        <v>3.9698185031608997E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>174450</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
+        <v>12506232.73</v>
+      </c>
+      <c r="D22" s="2">
         <v>21102</v>
       </c>
-      <c r="D22" s="2">
+      <c r="E22" s="2">
         <v>31533</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>49035</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <f t="shared" si="1"/>
         <v>52635</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>19840</v>
       </c>
-      <c r="H22" s="10">
+      <c r="I22" s="10">
         <v>131940</v>
       </c>
-      <c r="I22" s="10">
+      <c r="J22" s="10">
         <v>26050</v>
       </c>
-      <c r="J22" s="10">
+      <c r="K22" s="10">
         <v>12190</v>
       </c>
-      <c r="K22" s="10">
+      <c r="L22" s="10">
         <v>4270</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>85940</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>88520</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O22" s="16">
+        <f t="shared" si="2"/>
+        <v>0.11372886213814846</v>
+      </c>
+      <c r="P22" s="16">
+        <f t="shared" si="3"/>
+        <v>0.75631986242476357</v>
+      </c>
+      <c r="Q22" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49263399254800805</v>
+      </c>
+      <c r="R22" s="16">
+        <f t="shared" si="5"/>
+        <v>6.9876755517340211E-2</v>
+      </c>
+      <c r="S22" s="16">
+        <f t="shared" si="6"/>
+        <v>2.4476927486385785E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B23">
         <v>95930</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
+        <v>35789538.979999997</v>
+      </c>
+      <c r="D23" s="2">
         <v>12670</v>
       </c>
-      <c r="D23" s="2">
+      <c r="E23" s="2">
         <v>16608</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>31259</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <f t="shared" si="1"/>
         <v>29278</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>26570</v>
       </c>
-      <c r="H23" s="10">
+      <c r="I23" s="10">
         <v>78220</v>
       </c>
-      <c r="I23" s="10">
+      <c r="J23" s="10">
         <v>6940</v>
       </c>
-      <c r="J23" s="10">
+      <c r="K23" s="10">
         <v>7060</v>
       </c>
-      <c r="K23" s="10">
+      <c r="L23" s="10">
         <v>3710</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>45120</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>50820</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O23" s="16">
+        <f t="shared" si="2"/>
+        <v>0.27697279266131553</v>
+      </c>
+      <c r="P23" s="16">
+        <f t="shared" si="3"/>
+        <v>0.81538621911810694</v>
+      </c>
+      <c r="Q23" s="16">
+        <f t="shared" si="4"/>
+        <v>0.47034295840717188</v>
+      </c>
+      <c r="R23" s="16">
+        <f t="shared" si="5"/>
+        <v>7.359532992807255E-2</v>
+      </c>
+      <c r="S23" s="16">
+        <f t="shared" si="6"/>
+        <v>3.8674033149171269E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>10070</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
+        <v>1475697.9650000001</v>
+      </c>
+      <c r="D24" s="2">
         <v>600</v>
       </c>
-      <c r="D24" s="2">
+      <c r="E24" s="2">
         <v>2803</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>0</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <f t="shared" si="1"/>
         <v>3403</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>1900</v>
       </c>
-      <c r="H24" s="10">
+      <c r="I24" s="10">
         <v>7020</v>
       </c>
-      <c r="I24" s="10">
+      <c r="J24" s="10">
         <v>90</v>
       </c>
-      <c r="J24" s="10">
+      <c r="K24" s="10">
         <v>1500</v>
       </c>
-      <c r="K24" s="10">
+      <c r="L24" s="10">
         <v>1460</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>4620</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>5450</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O24" s="16">
+        <f t="shared" si="2"/>
+        <v>0.18867924528301888</v>
+      </c>
+      <c r="P24" s="16">
+        <f t="shared" si="3"/>
+        <v>0.69712015888778545</v>
+      </c>
+      <c r="Q24" s="16">
+        <f t="shared" si="4"/>
+        <v>0.45878848063555117</v>
+      </c>
+      <c r="R24" s="16">
+        <f t="shared" si="5"/>
+        <v>0.14895729890764647</v>
+      </c>
+      <c r="S24" s="16">
+        <f t="shared" si="6"/>
+        <v>0.14498510427010924</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>102640</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
+        <v>18058884.27</v>
+      </c>
+      <c r="D25" s="2">
         <v>13667</v>
       </c>
-      <c r="D25" s="2">
+      <c r="E25" s="2">
         <v>16668</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>28584</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <f t="shared" si="1"/>
         <v>30335</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>14700</v>
       </c>
-      <c r="H25" s="10">
+      <c r="I25" s="10">
         <v>72910</v>
       </c>
-      <c r="I25" s="10">
+      <c r="J25" s="10">
         <v>16680</v>
       </c>
-      <c r="J25" s="10">
+      <c r="K25" s="10">
         <v>9360</v>
       </c>
-      <c r="K25" s="10">
+      <c r="L25" s="10">
         <v>3680</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>50710</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>51930</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O25" s="16">
+        <f t="shared" si="2"/>
+        <v>0.14321901792673422</v>
+      </c>
+      <c r="P25" s="16">
+        <f t="shared" si="3"/>
+        <v>0.71034684333593145</v>
+      </c>
+      <c r="Q25" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49405689789555729</v>
+      </c>
+      <c r="R25" s="16">
+        <f t="shared" si="5"/>
+        <v>9.1192517537022608E-2</v>
+      </c>
+      <c r="S25" s="16">
+        <f t="shared" si="6"/>
+        <v>3.5853468433359313E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>249370</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
+        <v>10603045.039999999</v>
+      </c>
+      <c r="D26" s="2">
         <v>29774</v>
       </c>
-      <c r="D26" s="2">
+      <c r="E26" s="2">
         <v>43980</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>68180</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <f t="shared" si="1"/>
         <v>73754</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>37870</v>
       </c>
-      <c r="H26" s="10">
+      <c r="I26" s="10">
         <v>192870</v>
       </c>
-      <c r="I26" s="10">
+      <c r="J26" s="10">
         <v>28560</v>
       </c>
-      <c r="J26" s="10">
+      <c r="K26" s="10">
         <v>21690</v>
       </c>
-      <c r="K26" s="10">
+      <c r="L26" s="10">
         <v>6240</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>122480</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>126890</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O26" s="16">
+        <f t="shared" si="2"/>
+        <v>0.15186269398885191</v>
+      </c>
+      <c r="P26" s="16">
+        <f t="shared" si="3"/>
+        <v>0.77342904118378308</v>
+      </c>
+      <c r="Q26" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49115771744796888</v>
+      </c>
+      <c r="R26" s="16">
+        <f t="shared" si="5"/>
+        <v>8.6979187552632634E-2</v>
+      </c>
+      <c r="S26" s="16">
+        <f t="shared" si="6"/>
+        <v>2.50230581064282E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B27">
         <v>116900</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
+        <v>10100540.689999999</v>
+      </c>
+      <c r="D27" s="2">
         <v>11615</v>
       </c>
-      <c r="D27" s="2">
+      <c r="E27" s="2">
         <v>21153</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>22085</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <f t="shared" si="1"/>
         <v>32768</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>32590</v>
       </c>
-      <c r="H27" s="10">
+      <c r="I27" s="10">
         <v>98770</v>
       </c>
-      <c r="I27" s="10">
+      <c r="J27" s="10">
         <v>4860</v>
       </c>
-      <c r="J27" s="10">
+      <c r="K27" s="10">
         <v>10250</v>
       </c>
-      <c r="K27" s="10">
+      <c r="L27" s="10">
         <v>3020</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>56370</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>60530</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O27" s="16">
+        <f t="shared" si="2"/>
+        <v>0.27878528656971768</v>
+      </c>
+      <c r="P27" s="16">
+        <f t="shared" si="3"/>
+        <v>0.84491017964071857</v>
+      </c>
+      <c r="Q27" s="16">
+        <f t="shared" si="4"/>
+        <v>0.48220701454234388</v>
+      </c>
+      <c r="R27" s="16">
+        <f t="shared" si="5"/>
+        <v>8.7681779298545759E-2</v>
+      </c>
+      <c r="S27" s="16">
+        <f t="shared" si="6"/>
+        <v>2.5834046193327631E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B28">
         <v>259900</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
+        <v>30676070.77</v>
+      </c>
+      <c r="D28" s="2">
         <v>32006</v>
       </c>
-      <c r="D28" s="2">
+      <c r="E28" s="2">
         <v>42045</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>72846</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <f t="shared" si="1"/>
         <v>74051</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>59620</v>
       </c>
-      <c r="H28" s="10">
+      <c r="I28" s="10">
         <v>173660</v>
       </c>
-      <c r="I28" s="10">
+      <c r="J28" s="10">
         <v>56570</v>
       </c>
-      <c r="J28" s="10">
+      <c r="K28" s="10">
         <v>21700</v>
       </c>
-      <c r="K28" s="10">
+      <c r="L28" s="10">
         <v>7970</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>127000</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>132900</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O28" s="16">
+        <f t="shared" si="2"/>
+        <v>0.2293959215082724</v>
+      </c>
+      <c r="P28" s="16">
+        <f t="shared" si="3"/>
+        <v>0.66818006925740669</v>
+      </c>
+      <c r="Q28" s="16">
+        <f t="shared" si="4"/>
+        <v>0.48864948056944979</v>
+      </c>
+      <c r="R28" s="16">
+        <f t="shared" si="5"/>
+        <v>8.3493651404386304E-2</v>
+      </c>
+      <c r="S28" s="16">
+        <f t="shared" si="6"/>
+        <v>3.0665640631011928E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B29">
         <v>21810</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
+        <v>7552299.2810000004</v>
+      </c>
+      <c r="D29" s="2">
         <v>973</v>
       </c>
-      <c r="D29" s="2">
+      <c r="E29" s="2">
         <v>5754</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>187</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <f t="shared" si="1"/>
         <v>6727</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>4460</v>
       </c>
-      <c r="H29" s="10">
+      <c r="I29" s="10">
         <v>16270</v>
       </c>
-      <c r="I29" s="10">
+      <c r="J29" s="10">
         <v>240</v>
       </c>
-      <c r="J29" s="10">
+      <c r="K29" s="10">
         <v>2200</v>
       </c>
-      <c r="K29" s="10">
+      <c r="L29" s="10">
         <v>3090</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>10100</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>11700</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O29" s="16">
+        <f t="shared" si="2"/>
+        <v>0.20449335167354424</v>
+      </c>
+      <c r="P29" s="16">
+        <f t="shared" si="3"/>
+        <v>0.74598807886290697</v>
+      </c>
+      <c r="Q29" s="16">
+        <f t="shared" si="4"/>
+        <v>0.46309032553874369</v>
+      </c>
+      <c r="R29" s="16">
+        <f t="shared" si="5"/>
+        <v>0.10087116001834021</v>
+      </c>
+      <c r="S29" s="16">
+        <f t="shared" si="6"/>
+        <v>0.14167812929848694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30">
         <v>121850</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
+        <v>8180210.3660000004</v>
+      </c>
+      <c r="D30" s="2">
         <v>17718</v>
       </c>
-      <c r="D30" s="2">
+      <c r="E30" s="2">
         <v>19147</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>39272</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <f t="shared" si="1"/>
         <v>36865</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>34950</v>
       </c>
-      <c r="H30" s="10">
+      <c r="I30" s="10">
         <v>101320</v>
       </c>
-      <c r="I30" s="10">
+      <c r="J30" s="10">
         <v>8410</v>
       </c>
-      <c r="J30" s="10">
+      <c r="K30" s="10">
         <v>8590</v>
       </c>
-      <c r="K30" s="10">
+      <c r="L30" s="10">
         <v>3530</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>57890</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>63960</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O30" s="16">
+        <f t="shared" si="2"/>
+        <v>0.28682806729585558</v>
+      </c>
+      <c r="P30" s="16">
+        <f t="shared" si="3"/>
+        <v>0.83151415675010254</v>
+      </c>
+      <c r="Q30" s="16">
+        <f t="shared" si="4"/>
+        <v>0.47509232663110379</v>
+      </c>
+      <c r="R30" s="16">
+        <f t="shared" si="5"/>
+        <v>7.049651210504719E-2</v>
+      </c>
+      <c r="S30" s="16">
+        <f t="shared" si="6"/>
+        <v>2.8970045137464095E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B31">
         <v>255130</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
+        <v>15619408.300000001</v>
+      </c>
+      <c r="D31" s="2">
         <v>35716</v>
       </c>
-      <c r="D31" s="2">
+      <c r="E31" s="2">
         <v>35993</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>72965</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <f t="shared" si="1"/>
         <v>71709</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>41480</v>
       </c>
-      <c r="H31" s="10">
+      <c r="I31" s="10">
         <v>155360</v>
       </c>
-      <c r="I31" s="10">
+      <c r="J31" s="10">
         <v>65480</v>
       </c>
-      <c r="J31" s="10">
+      <c r="K31" s="10">
         <v>28240</v>
       </c>
-      <c r="K31" s="10">
+      <c r="L31" s="10">
         <v>6060</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>127990</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>127150</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O31" s="16">
+        <f t="shared" si="2"/>
+        <v>0.1625837808176224</v>
+      </c>
+      <c r="P31" s="16">
+        <f t="shared" si="3"/>
+        <v>0.60894445968721833</v>
+      </c>
+      <c r="Q31" s="16">
+        <f t="shared" si="4"/>
+        <v>0.50166581742641003</v>
+      </c>
+      <c r="R31" s="16">
+        <f t="shared" si="5"/>
+        <v>0.11068866852193</v>
+      </c>
+      <c r="S31" s="16">
+        <f t="shared" si="6"/>
+        <v>2.3752596715399994E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <v>221610</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
+        <v>21011029.079999998</v>
+      </c>
+      <c r="D32" s="2">
         <v>34738</v>
       </c>
-      <c r="D32" s="2">
+      <c r="E32" s="2">
         <v>31966</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>66773</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <f t="shared" si="1"/>
         <v>66704</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>44690</v>
       </c>
-      <c r="H32" s="10">
+      <c r="I32" s="10">
         <v>153160</v>
       </c>
-      <c r="I32" s="10">
+      <c r="J32" s="10">
         <v>40390</v>
       </c>
-      <c r="J32" s="10">
+      <c r="K32" s="10">
         <v>21950</v>
       </c>
-      <c r="K32" s="10">
+      <c r="L32" s="10">
         <v>6110</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>109470</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>112140</v>
+      </c>
+      <c r="O32" s="16">
+        <f t="shared" si="2"/>
+        <v>0.20166057488380487</v>
+      </c>
+      <c r="P32" s="16">
+        <f t="shared" si="3"/>
+        <v>0.69112404674879291</v>
+      </c>
+      <c r="Q32" s="16">
+        <f t="shared" si="4"/>
+        <v>0.49397590361445781</v>
+      </c>
+      <c r="R32" s="16">
+        <f t="shared" si="5"/>
+        <v>9.9047876900861878E-2</v>
+      </c>
+      <c r="S32" s="16">
+        <f t="shared" si="6"/>
+        <v>2.7570957989260413E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added in density attributes and cross-checked total values
</commit_message>
<xml_diff>
--- a/Data/Combined Attributes.xlsx
+++ b/Data/Combined Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yi Zhen\Documents\GitHub\BT4015\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC98B23-209E-41CD-B8A3-9E15E153D28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B38CCE-A048-4453-967F-E80BDD2DA9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="830" yWindow="230" windowWidth="18320" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-450" yWindow="0" windowWidth="19020" windowHeight="9880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Planning Area of Residence</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Population</t>
   </si>
   <si>
-    <t>Houesholds Below Median Income</t>
-  </si>
-  <si>
     <t xml:space="preserve">Households Above Median Income </t>
   </si>
   <si>
@@ -184,6 +181,30 @@
   </si>
   <si>
     <t>Others Ratio</t>
+  </si>
+  <si>
+    <t>Households Below Median Income</t>
+  </si>
+  <si>
+    <t>Male Ratio</t>
+  </si>
+  <si>
+    <t>Female Ratio</t>
+  </si>
+  <si>
+    <t>Population Density</t>
+  </si>
+  <si>
+    <t>Households Below Median Income Density</t>
+  </si>
+  <si>
+    <t>Households Above Median Income Density</t>
+  </si>
+  <si>
+    <t>HDB Housing Density</t>
+  </si>
+  <si>
+    <t>Private Housing Density</t>
   </si>
 </sst>
 </file>
@@ -213,18 +234,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -274,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -288,11 +303,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -306,6 +317,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S32"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,29 +616,35 @@
     <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.36328125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.90625" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" style="7" customWidth="1"/>
+    <col min="10" max="12" width="9.36328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="36.90625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="37.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>44</v>
+      <c r="C1" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>33</v>
@@ -632,117 +652,170 @@
       <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="15" t="s">
-        <v>49</v>
+      <c r="T1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="12">
         <f t="shared" ref="B2:L2" si="0">SUM(B3:B32)</f>
         <v>4010200</v>
       </c>
-      <c r="D2" s="8">
+      <c r="C2" s="12">
+        <f>SUM(C3:C32)</f>
+        <v>453.63192689900001</v>
+      </c>
+      <c r="D2" s="14">
         <f t="shared" si="0"/>
         <v>516681</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="14">
         <f t="shared" si="0"/>
         <v>662911</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="12">
         <f t="shared" si="0"/>
         <v>1075957</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="12">
         <f t="shared" si="0"/>
         <v>1179592</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="12">
         <f t="shared" si="0"/>
         <v>891370</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="15">
         <f t="shared" si="0"/>
         <v>2982590</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="15">
         <f t="shared" si="0"/>
         <v>544020</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="15">
         <f t="shared" si="0"/>
         <v>357670</v>
       </c>
-      <c r="L2" s="11">
+      <c r="L2" s="15">
         <f t="shared" si="0"/>
         <v>125910</v>
       </c>
-      <c r="M2" s="9">
-        <f>SUM(M4:M32)</f>
-        <v>1883410</v>
-      </c>
-      <c r="N2" s="9">
+      <c r="M2" s="12">
+        <f>SUM(M3:M32)</f>
+        <v>1960980</v>
+      </c>
+      <c r="N2" s="12">
         <f>SUM(N3:N32)</f>
         <v>2049270</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="12">
         <f>H2/B2</f>
         <v>0.22227569697271957</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="12">
         <f>I2/B2</f>
         <v>0.74375093511545554</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="12">
         <f>M2/B2</f>
-        <v>0.46965488005585754</v>
-      </c>
-      <c r="R2" s="9">
+        <v>0.48899805495985238</v>
+      </c>
+      <c r="R2" s="12">
         <f>K2/B2</f>
         <v>8.9190065333399834E-2</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="12">
         <f>L2/B2</f>
         <v>3.139743653683108E-2</v>
       </c>
+      <c r="T2" s="12">
+        <f>M2/B2</f>
+        <v>0.48899805495985238</v>
+      </c>
+      <c r="U2" s="12">
+        <f>N2/B2</f>
+        <v>0.5110144132462221</v>
+      </c>
+      <c r="V2" s="12">
+        <f>B2/C2</f>
+        <v>8840.2067010879964</v>
+      </c>
+      <c r="W2" s="12">
+        <f>D2/C2</f>
+        <v>1138.9872920365187</v>
+      </c>
+      <c r="X2" s="12">
+        <f>E2/C2</f>
+        <v>1461.3411461834683</v>
+      </c>
+      <c r="Y2" s="12">
+        <f>F2/C2</f>
+        <v>2371.8722960157943</v>
+      </c>
+      <c r="Z2" s="12">
+        <f>G2/C2</f>
+        <v>2600.3284382199872</v>
+      </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -750,7 +823,7 @@
         <v>162280</v>
       </c>
       <c r="C3">
-        <v>13942583.369999999</v>
+        <v>13.942583369999999</v>
       </c>
       <c r="D3" s="2">
         <v>25513</v>
@@ -768,16 +841,16 @@
       <c r="H3">
         <v>47950</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <v>134350</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="7">
         <v>11140</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="7">
         <v>12810</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>3970</v>
       </c>
       <c r="M3">
@@ -786,28 +859,56 @@
       <c r="N3">
         <v>84700</v>
       </c>
-      <c r="O3" s="16">
+      <c r="O3" s="12">
         <f t="shared" ref="O3:O32" si="2">H3/B3</f>
         <v>0.29547695341385261</v>
       </c>
-      <c r="P3" s="16">
+      <c r="P3" s="12">
         <f t="shared" ref="P3:P32" si="3">I3/B3</f>
         <v>0.8278900665516391</v>
       </c>
-      <c r="Q3" s="16">
+      <c r="Q3" s="12">
         <f t="shared" ref="Q3:Q32" si="4">M3/B3</f>
         <v>0.47800098595020951</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="12">
         <f t="shared" ref="R3:R32" si="5">K3/B3</f>
         <v>7.8937638649248215E-2</v>
       </c>
-      <c r="S3" s="16">
+      <c r="S3" s="12">
         <f t="shared" ref="S3:S32" si="6">L3/B3</f>
         <v>2.4463889573576536E-2</v>
       </c>
+      <c r="T3" s="12">
+        <f t="shared" ref="T3:T32" si="7">M3/B3</f>
+        <v>0.47800098595020951</v>
+      </c>
+      <c r="U3" s="12">
+        <f t="shared" ref="U3:U32" si="8">N3/B3</f>
+        <v>0.52193739216169588</v>
+      </c>
+      <c r="V3" s="12">
+        <f t="shared" ref="V3:V32" si="9">B3/C3</f>
+        <v>11639.162965248957</v>
+      </c>
+      <c r="W3" s="12">
+        <f t="shared" ref="W3:W32" si="10">D3/C3</f>
+        <v>1829.8617496450374</v>
+      </c>
+      <c r="X3" s="12">
+        <f t="shared" ref="X3:X32" si="11">E3/C3</f>
+        <v>1667.5532347919539</v>
+      </c>
+      <c r="Y3" s="12">
+        <f t="shared" ref="Y3:Y32" si="12">F3/C3</f>
+        <v>3632.5405884949714</v>
+      </c>
+      <c r="Z3" s="12">
+        <f t="shared" ref="Z3:Z32" si="13">G3/C3</f>
+        <v>3497.4149844369913</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -815,7 +916,7 @@
         <v>276990</v>
       </c>
       <c r="C4">
-        <v>48665179.850000001</v>
+        <v>48.665179850000001</v>
       </c>
       <c r="D4" s="2">
         <v>36087</v>
@@ -833,16 +934,16 @@
       <c r="H4">
         <v>75230</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="7">
         <v>201780</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="7">
         <v>39300</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="7">
         <v>24450</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="7">
         <v>11470</v>
       </c>
       <c r="M4">
@@ -851,28 +952,56 @@
       <c r="N4">
         <v>142790</v>
       </c>
-      <c r="O4" s="16">
+      <c r="O4" s="12">
         <f t="shared" si="2"/>
         <v>0.27159825264449983</v>
       </c>
-      <c r="P4" s="16">
+      <c r="P4" s="12">
         <f t="shared" si="3"/>
         <v>0.72847395212823562</v>
       </c>
-      <c r="Q4" s="16">
+      <c r="Q4" s="12">
         <f t="shared" si="4"/>
         <v>0.48453012744142387</v>
       </c>
-      <c r="R4" s="16">
+      <c r="R4" s="12">
         <f t="shared" si="5"/>
         <v>8.8270334669121625E-2</v>
       </c>
-      <c r="S4" s="16">
+      <c r="S4" s="12">
         <f t="shared" si="6"/>
         <v>4.1409437163796525E-2</v>
       </c>
+      <c r="T4" s="12">
+        <f t="shared" si="7"/>
+        <v>0.48453012744142387</v>
+      </c>
+      <c r="U4" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51550597494494388</v>
+      </c>
+      <c r="V4" s="12">
+        <f t="shared" si="9"/>
+        <v>5691.7492312524555</v>
+      </c>
+      <c r="W4" s="12">
+        <f t="shared" si="10"/>
+        <v>741.53635332758358</v>
+      </c>
+      <c r="X4" s="12">
+        <f t="shared" si="11"/>
+        <v>917.45268665641231</v>
+      </c>
+      <c r="Y4" s="12">
+        <f t="shared" si="12"/>
+        <v>1326.7186148085302</v>
+      </c>
+      <c r="Z4" s="12">
+        <f t="shared" si="13"/>
+        <v>1658.9890399839958</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -880,7 +1009,7 @@
         <v>87320</v>
       </c>
       <c r="C5">
-        <v>7608112.5300000003</v>
+        <v>7.6081125300000005</v>
       </c>
       <c r="D5" s="2">
         <v>8259</v>
@@ -898,16 +1027,16 @@
       <c r="H5">
         <v>23170</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="7">
         <v>75040</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="7">
         <v>3190</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="7">
         <v>6490</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="7">
         <v>2590</v>
       </c>
       <c r="M5">
@@ -916,28 +1045,56 @@
       <c r="N5">
         <v>45060</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="12">
         <f t="shared" si="2"/>
         <v>0.26534585432890517</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="12">
         <f t="shared" si="3"/>
         <v>0.85936784241868991</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="12">
         <f t="shared" si="4"/>
         <v>0.48396701786532292</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5" s="12">
         <f t="shared" si="5"/>
         <v>7.4324324324324328E-2</v>
       </c>
-      <c r="S5" s="16">
+      <c r="S5" s="12">
         <f t="shared" si="6"/>
         <v>2.9661016949152543E-2</v>
       </c>
+      <c r="T5" s="12">
+        <f t="shared" si="7"/>
+        <v>0.48396701786532292</v>
+      </c>
+      <c r="U5" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51603298213467708</v>
+      </c>
+      <c r="V5" s="12">
+        <f t="shared" si="9"/>
+        <v>11477.222459011131</v>
+      </c>
+      <c r="W5" s="12">
+        <f t="shared" si="10"/>
+        <v>1085.5517669373903</v>
+      </c>
+      <c r="X5" s="12">
+        <f t="shared" si="11"/>
+        <v>2204.6203882843988</v>
+      </c>
+      <c r="Y5" s="12">
+        <f t="shared" si="12"/>
+        <v>2700.669833546744</v>
+      </c>
+      <c r="Z5" s="12">
+        <f t="shared" si="13"/>
+        <v>3290.1721552217891</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -945,7 +1102,7 @@
         <v>158030</v>
       </c>
       <c r="C6">
-        <v>11140156.279999999</v>
+        <v>11.140156279999999</v>
       </c>
       <c r="D6" s="2">
         <v>22192</v>
@@ -963,16 +1120,16 @@
       <c r="H6">
         <v>33420</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="7">
         <v>113460</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="7">
         <v>25240</v>
       </c>
-      <c r="K6" s="10">
+      <c r="K6" s="7">
         <v>14950</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="7">
         <v>4380</v>
       </c>
       <c r="M6">
@@ -981,28 +1138,56 @@
       <c r="N6">
         <v>80550</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6" s="12">
         <f t="shared" si="2"/>
         <v>0.21147883313294943</v>
       </c>
-      <c r="P6" s="16">
+      <c r="P6" s="12">
         <f t="shared" si="3"/>
         <v>0.71796494336518379</v>
       </c>
-      <c r="Q6" s="16">
+      <c r="Q6" s="12">
         <f t="shared" si="4"/>
         <v>0.49028665443270264</v>
       </c>
-      <c r="R6" s="16">
+      <c r="R6" s="12">
         <f t="shared" si="5"/>
         <v>9.4602290704296654E-2</v>
       </c>
-      <c r="S6" s="16">
+      <c r="S6" s="12">
         <f t="shared" si="6"/>
         <v>2.7716256407011326E-2</v>
       </c>
+      <c r="T6" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49028665443270264</v>
+      </c>
+      <c r="U6" s="12">
+        <f t="shared" si="8"/>
+        <v>0.5097133455672973</v>
+      </c>
+      <c r="V6" s="12">
+        <f t="shared" si="9"/>
+        <v>14185.617869985574</v>
+      </c>
+      <c r="W6" s="12">
+        <f t="shared" si="10"/>
+        <v>1992.0725923604368</v>
+      </c>
+      <c r="X6" s="12">
+        <f t="shared" si="11"/>
+        <v>2344.9401734963812</v>
+      </c>
+      <c r="Y6" s="12">
+        <f t="shared" si="12"/>
+        <v>3894.6491332346013</v>
+      </c>
+      <c r="Z6" s="12">
+        <f t="shared" si="13"/>
+        <v>4337.0127658568181</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1010,7 +1195,7 @@
         <v>151250</v>
       </c>
       <c r="C7">
-        <v>17774660.609999999</v>
+        <v>17.774660609999998</v>
       </c>
       <c r="D7" s="2">
         <v>22749</v>
@@ -1028,16 +1213,16 @@
       <c r="H7">
         <v>44420</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="7">
         <v>120830</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="7">
         <v>11430</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="7">
         <v>13980</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="7">
         <v>5010</v>
       </c>
       <c r="M7">
@@ -1046,28 +1231,56 @@
       <c r="N7">
         <v>78520</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="12">
         <f t="shared" si="2"/>
         <v>0.29368595041322315</v>
       </c>
-      <c r="P7" s="16">
+      <c r="P7" s="12">
         <f t="shared" si="3"/>
         <v>0.79887603305785126</v>
       </c>
-      <c r="Q7" s="16">
+      <c r="Q7" s="12">
         <f t="shared" si="4"/>
         <v>0.48085950413223139</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="12">
         <f t="shared" si="5"/>
         <v>9.24297520661157E-2</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="12">
         <f t="shared" si="6"/>
         <v>3.312396694214876E-2</v>
       </c>
+      <c r="T7" s="12">
+        <f t="shared" si="7"/>
+        <v>0.48085950413223139</v>
+      </c>
+      <c r="U7" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51914049586776856</v>
+      </c>
+      <c r="V7" s="12">
+        <f t="shared" si="9"/>
+        <v>8509.3045273059652</v>
+      </c>
+      <c r="W7" s="12">
+        <f t="shared" si="10"/>
+        <v>1279.8556607714606</v>
+      </c>
+      <c r="X7" s="12">
+        <f t="shared" si="11"/>
+        <v>1378.8167626791048</v>
+      </c>
+      <c r="Y7" s="12">
+        <f t="shared" si="12"/>
+        <v>3031.0002076602241</v>
+      </c>
+      <c r="Z7" s="12">
+        <f t="shared" si="13"/>
+        <v>2658.6724234505655</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1075,7 +1288,7 @@
         <v>138270</v>
       </c>
       <c r="C8">
-        <v>9019929.7300000004</v>
+        <v>9.0199297300000012</v>
       </c>
       <c r="D8" s="2">
         <v>17434</v>
@@ -1093,16 +1306,16 @@
       <c r="H8">
         <v>27890</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="7">
         <v>102800</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="7">
         <v>21690</v>
       </c>
-      <c r="K8" s="10">
+      <c r="K8" s="7">
         <v>10340</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="7">
         <v>3450</v>
       </c>
       <c r="M8">
@@ -1111,28 +1324,56 @@
       <c r="N8">
         <v>70120</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="12">
         <f t="shared" si="2"/>
         <v>0.20170680552542128</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="12">
         <f t="shared" si="3"/>
         <v>0.74347291531062409</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="12">
         <f t="shared" si="4"/>
         <v>0.49287625659940698</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="12">
         <f t="shared" si="5"/>
         <v>7.4781225139220364E-2</v>
       </c>
-      <c r="S8" s="16">
+      <c r="S8" s="12">
         <f t="shared" si="6"/>
         <v>2.495118246908223E-2</v>
       </c>
+      <c r="T8" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49287625659940698</v>
+      </c>
+      <c r="U8" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50712374340059307</v>
+      </c>
+      <c r="V8" s="12">
+        <f t="shared" si="9"/>
+        <v>15329.387715751083</v>
+      </c>
+      <c r="W8" s="12">
+        <f t="shared" si="10"/>
+        <v>1932.831022176932</v>
+      </c>
+      <c r="X8" s="12">
+        <f t="shared" si="11"/>
+        <v>2411.9921830034032</v>
+      </c>
+      <c r="Y8" s="12">
+        <f t="shared" si="12"/>
+        <v>4004.4657864535266</v>
+      </c>
+      <c r="Z8" s="12">
+        <f t="shared" si="13"/>
+        <v>4344.8232051803352</v>
+      </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1140,7 +1381,7 @@
         <v>77860</v>
       </c>
       <c r="C9">
-        <v>17514936.539999999</v>
+        <v>17.514936540000001</v>
       </c>
       <c r="D9" s="2">
         <v>3610</v>
@@ -1158,16 +1399,16 @@
       <c r="H9">
         <v>18040</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="7">
         <v>67400</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="7">
         <v>640</v>
       </c>
-      <c r="K9" s="10">
+      <c r="K9" s="7">
         <v>3840</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="7">
         <v>5980</v>
       </c>
       <c r="M9">
@@ -1176,28 +1417,56 @@
       <c r="N9">
         <v>41880</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="12">
         <f t="shared" si="2"/>
         <v>0.23169791934240946</v>
       </c>
-      <c r="P9" s="16">
+      <c r="P9" s="12">
         <f t="shared" si="3"/>
         <v>0.86565630619059852</v>
       </c>
-      <c r="Q9" s="16">
+      <c r="Q9" s="12">
         <f t="shared" si="4"/>
         <v>0.46211148214744413</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="12">
         <f t="shared" si="5"/>
         <v>4.9319291035191372E-2</v>
       </c>
-      <c r="S9" s="16">
+      <c r="S9" s="12">
         <f t="shared" si="6"/>
         <v>7.6804520935011555E-2</v>
       </c>
+      <c r="T9" s="12">
+        <f t="shared" si="7"/>
+        <v>0.46211148214744413</v>
+      </c>
+      <c r="U9" s="12">
+        <f t="shared" si="8"/>
+        <v>0.53788851785255587</v>
+      </c>
+      <c r="V9" s="12">
+        <f t="shared" si="9"/>
+        <v>4445.3486783800818</v>
+      </c>
+      <c r="W9" s="12">
+        <f t="shared" si="10"/>
+        <v>206.10979615915866</v>
+      </c>
+      <c r="X9" s="12">
+        <f t="shared" si="11"/>
+        <v>979.50683183006265</v>
+      </c>
+      <c r="Y9" s="12">
+        <f t="shared" si="12"/>
+        <v>142.33565701517523</v>
+      </c>
+      <c r="Z9" s="12">
+        <f t="shared" si="13"/>
+        <v>1185.6166279892213</v>
+      </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1474,7 @@
         <v>192070</v>
       </c>
       <c r="C10">
-        <v>6117280.0489999996</v>
+        <v>6.1172800489999997</v>
       </c>
       <c r="D10" s="2">
         <v>21847</v>
@@ -1223,16 +1492,16 @@
       <c r="H10">
         <v>32830</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="7">
         <v>133520</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="7">
         <v>35500</v>
       </c>
-      <c r="K10" s="10">
+      <c r="K10" s="7">
         <v>18020</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="7">
         <v>5020</v>
       </c>
       <c r="M10">
@@ -1241,28 +1510,56 @@
       <c r="N10">
         <v>96380</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="12">
         <f t="shared" si="2"/>
         <v>0.17092726610090073</v>
       </c>
-      <c r="P10" s="16">
+      <c r="P10" s="12">
         <f t="shared" si="3"/>
         <v>0.69516322174207323</v>
       </c>
-      <c r="Q10" s="16">
+      <c r="Q10" s="12">
         <f t="shared" si="4"/>
         <v>0.49820377987192171</v>
       </c>
-      <c r="R10" s="16">
+      <c r="R10" s="12">
         <f t="shared" si="5"/>
         <v>9.3819961472379865E-2</v>
       </c>
-      <c r="S10" s="16">
+      <c r="S10" s="12">
         <f t="shared" si="6"/>
         <v>2.6136304472327797E-2</v>
       </c>
+      <c r="T10" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49820377987192171</v>
+      </c>
+      <c r="U10" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50179622012807834</v>
+      </c>
+      <c r="V10" s="12">
+        <f t="shared" si="9"/>
+        <v>31397.941317301298</v>
+      </c>
+      <c r="W10" s="12">
+        <f t="shared" si="10"/>
+        <v>3571.3584836730433</v>
+      </c>
+      <c r="X10" s="12">
+        <f t="shared" si="11"/>
+        <v>5184.3302490596834</v>
+      </c>
+      <c r="Y10" s="12">
+        <f t="shared" si="12"/>
+        <v>8176.5097558638845</v>
+      </c>
+      <c r="Z10" s="12">
+        <f t="shared" si="13"/>
+        <v>8755.6887327327277</v>
+      </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1270,7 +1567,7 @@
         <v>91990</v>
       </c>
       <c r="C11">
-        <v>9524177.7479999997</v>
+        <v>9.5241777479999996</v>
       </c>
       <c r="D11" s="2">
         <v>11433</v>
@@ -1288,16 +1585,16 @@
       <c r="H11">
         <v>24700</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="7">
         <v>73630</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="7">
         <v>8270</v>
       </c>
-      <c r="K11" s="10">
+      <c r="K11" s="7">
         <v>6970</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="7">
         <v>3120</v>
       </c>
       <c r="M11">
@@ -1306,28 +1603,56 @@
       <c r="N11">
         <v>48360</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11" s="12">
         <f t="shared" si="2"/>
         <v>0.26850744646157193</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="12">
         <f t="shared" si="3"/>
         <v>0.80041308837917169</v>
       </c>
-      <c r="Q11" s="16">
+      <c r="Q11" s="12">
         <f t="shared" si="4"/>
         <v>0.47429068376997502</v>
       </c>
-      <c r="R11" s="16">
+      <c r="R11" s="12">
         <f t="shared" si="5"/>
         <v>7.5769105337536682E-2</v>
       </c>
-      <c r="S11" s="16">
+      <c r="S11" s="12">
         <f t="shared" si="6"/>
         <v>3.3916730079356451E-2</v>
       </c>
+      <c r="T11" s="12">
+        <f t="shared" si="7"/>
+        <v>0.47429068376997502</v>
+      </c>
+      <c r="U11" s="12">
+        <f t="shared" si="8"/>
+        <v>0.52570931623002504</v>
+      </c>
+      <c r="V11" s="12">
+        <f t="shared" si="9"/>
+        <v>9658.5765652386272</v>
+      </c>
+      <c r="W11" s="12">
+        <f t="shared" si="10"/>
+        <v>1200.4185875679229</v>
+      </c>
+      <c r="X11" s="12">
+        <f t="shared" si="11"/>
+        <v>1699.4642926943409</v>
+      </c>
+      <c r="Y11" s="12">
+        <f t="shared" si="12"/>
+        <v>2710.9951833292898</v>
+      </c>
+      <c r="Z11" s="12">
+        <f t="shared" si="13"/>
+        <v>2899.8828802622638</v>
+      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -1335,7 +1660,7 @@
         <v>3190</v>
       </c>
       <c r="C12">
-        <v>5083636.2889999999</v>
+        <v>5.0836362890000002</v>
       </c>
       <c r="D12" s="2">
         <v>260</v>
@@ -1353,16 +1678,16 @@
       <c r="H12">
         <v>630</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="7">
         <v>2500</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="7">
         <v>30</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12" s="7">
         <v>200</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="7">
         <v>460</v>
       </c>
       <c r="M12">
@@ -1371,28 +1696,56 @@
       <c r="N12">
         <v>1600</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12" s="12">
         <f t="shared" si="2"/>
         <v>0.19749216300940439</v>
       </c>
-      <c r="P12" s="16">
+      <c r="P12" s="12">
         <f t="shared" si="3"/>
         <v>0.78369905956112851</v>
       </c>
-      <c r="Q12" s="16">
+      <c r="Q12" s="12">
         <f t="shared" si="4"/>
         <v>0.49843260188087773</v>
       </c>
-      <c r="R12" s="16">
+      <c r="R12" s="12">
         <f t="shared" si="5"/>
         <v>6.2695924764890276E-2</v>
       </c>
-      <c r="S12" s="16">
+      <c r="S12" s="12">
         <f t="shared" si="6"/>
         <v>0.14420062695924765</v>
       </c>
+      <c r="T12" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49843260188087773</v>
+      </c>
+      <c r="U12" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50156739811912221</v>
+      </c>
+      <c r="V12" s="12">
+        <f t="shared" si="9"/>
+        <v>627.50358575072323</v>
+      </c>
+      <c r="W12" s="12">
+        <f t="shared" si="10"/>
+        <v>51.144492882504089</v>
+      </c>
+      <c r="X12" s="12">
+        <f t="shared" si="11"/>
+        <v>218.54435227870016</v>
+      </c>
+      <c r="Y12" s="12">
+        <f t="shared" si="12"/>
+        <v>45.046495654205522</v>
+      </c>
+      <c r="Z12" s="12">
+        <f t="shared" si="13"/>
+        <v>269.68884516120426</v>
+      </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1400,7 +1753,7 @@
         <v>110110</v>
       </c>
       <c r="C13">
-        <v>9644787.3660000004</v>
+        <v>9.644787366000001</v>
       </c>
       <c r="D13" s="2">
         <v>17907</v>
@@ -1418,16 +1771,16 @@
       <c r="H13">
         <v>30000</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="7">
         <v>85460</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="7">
         <v>12470</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="7">
         <v>8640</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="7">
         <v>3550</v>
       </c>
       <c r="M13">
@@ -1436,28 +1789,56 @@
       <c r="N13">
         <v>55860</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13" s="12">
         <f t="shared" si="2"/>
         <v>0.27245481790936338</v>
       </c>
-      <c r="P13" s="16">
+      <c r="P13" s="12">
         <f t="shared" si="3"/>
         <v>0.77613295795113979</v>
       </c>
-      <c r="Q13" s="16">
+      <c r="Q13" s="12">
         <f t="shared" si="4"/>
         <v>0.49277994732540187</v>
       </c>
-      <c r="R13" s="16">
+      <c r="R13" s="12">
         <f t="shared" si="5"/>
         <v>7.8466987557896647E-2</v>
       </c>
-      <c r="S13" s="16">
+      <c r="S13" s="12">
         <f t="shared" si="6"/>
         <v>3.2240486785941332E-2</v>
       </c>
+      <c r="T13" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49277994732540187</v>
+      </c>
+      <c r="U13" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50731087094723459</v>
+      </c>
+      <c r="V13" s="12">
+        <f t="shared" si="9"/>
+        <v>11416.529553379476</v>
+      </c>
+      <c r="W13" s="12">
+        <f t="shared" si="10"/>
+        <v>1856.6505740837913</v>
+      </c>
+      <c r="X13" s="12">
+        <f t="shared" si="11"/>
+        <v>1779.5104597643442</v>
+      </c>
+      <c r="Y13" s="12">
+        <f t="shared" si="12"/>
+        <v>3211.1646244456974</v>
+      </c>
+      <c r="Z13" s="12">
+        <f t="shared" si="13"/>
+        <v>3636.1610338481355</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -1465,7 +1846,7 @@
         <v>227560</v>
       </c>
       <c r="C14">
-        <v>13933022.85</v>
+        <v>13.93302285</v>
       </c>
       <c r="D14" s="2">
         <v>29848</v>
@@ -1483,16 +1864,16 @@
       <c r="H14">
         <v>55530</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="7">
         <v>184810</v>
       </c>
-      <c r="J14" s="10">
+      <c r="J14" s="7">
         <v>18760</v>
       </c>
-      <c r="K14" s="10">
+      <c r="K14" s="7">
         <v>18710</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="7">
         <v>5290</v>
       </c>
       <c r="M14">
@@ -1501,28 +1882,56 @@
       <c r="N14">
         <v>116070</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="12">
         <f t="shared" si="2"/>
         <v>0.2440235542274565</v>
       </c>
-      <c r="P14" s="16">
+      <c r="P14" s="12">
         <f t="shared" si="3"/>
         <v>0.81213745825276851</v>
       </c>
-      <c r="Q14" s="16">
+      <c r="Q14" s="12">
         <f t="shared" si="4"/>
         <v>0.4899367199859378</v>
       </c>
-      <c r="R14" s="16">
+      <c r="R14" s="12">
         <f t="shared" si="5"/>
         <v>8.2220073826683074E-2</v>
       </c>
-      <c r="S14" s="16">
+      <c r="S14" s="12">
         <f t="shared" si="6"/>
         <v>2.3246616277025841E-2</v>
       </c>
+      <c r="T14" s="12">
+        <f t="shared" si="7"/>
+        <v>0.4899367199859378</v>
+      </c>
+      <c r="U14" s="12">
+        <f t="shared" si="8"/>
+        <v>0.5100632800140622</v>
+      </c>
+      <c r="V14" s="12">
+        <f t="shared" si="9"/>
+        <v>16332.421359662092</v>
+      </c>
+      <c r="W14" s="12">
+        <f t="shared" si="10"/>
+        <v>2142.2486937211906</v>
+      </c>
+      <c r="X14" s="12">
+        <f t="shared" si="11"/>
+        <v>2638.3363033098017</v>
+      </c>
+      <c r="Y14" s="12">
+        <f t="shared" si="12"/>
+        <v>4161.2649763220616</v>
+      </c>
+      <c r="Z14" s="12">
+        <f t="shared" si="13"/>
+        <v>4780.5849970309919</v>
+      </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1530,7 +1939,7 @@
         <v>78600</v>
       </c>
       <c r="C15">
-        <v>22949603.41</v>
+        <v>22.949603410000002</v>
       </c>
       <c r="D15" s="2">
         <v>11653</v>
@@ -1548,16 +1957,16 @@
       <c r="H15">
         <v>21640</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="7">
         <v>55440</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>12700</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>8610</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="7">
         <v>1850</v>
       </c>
       <c r="M15">
@@ -1566,28 +1975,56 @@
       <c r="N15">
         <v>39670</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="12">
         <f t="shared" si="2"/>
         <v>0.27531806615776083</v>
       </c>
-      <c r="P15" s="16">
+      <c r="P15" s="12">
         <f t="shared" si="3"/>
         <v>0.70534351145038165</v>
       </c>
-      <c r="Q15" s="16">
+      <c r="Q15" s="12">
         <f t="shared" si="4"/>
         <v>0.49529262086513998</v>
       </c>
-      <c r="R15" s="16">
+      <c r="R15" s="12">
         <f t="shared" si="5"/>
         <v>0.10954198473282442</v>
       </c>
-      <c r="S15" s="16">
+      <c r="S15" s="12">
         <f t="shared" si="6"/>
         <v>2.3536895674300253E-2</v>
       </c>
+      <c r="T15" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49529262086513998</v>
+      </c>
+      <c r="U15" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50470737913486008</v>
+      </c>
+      <c r="V15" s="12">
+        <f t="shared" si="9"/>
+        <v>3424.8957855956255</v>
+      </c>
+      <c r="W15" s="12">
+        <f t="shared" si="10"/>
+        <v>507.76476577030309</v>
+      </c>
+      <c r="X15" s="12">
+        <f t="shared" si="11"/>
+        <v>492.60110504018508</v>
+      </c>
+      <c r="Y15" s="12">
+        <f t="shared" si="12"/>
+        <v>1074.0490613122975</v>
+      </c>
+      <c r="Z15" s="12">
+        <f t="shared" si="13"/>
+        <v>1000.3658708104881</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -1595,7 +2032,7 @@
         <v>262730</v>
       </c>
       <c r="C16">
-        <v>14680284.49</v>
+        <v>14.68028449</v>
       </c>
       <c r="D16" s="2">
         <v>35323</v>
@@ -1613,16 +2050,16 @@
       <c r="H16">
         <v>51550</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I16" s="7">
         <v>183590</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="7">
         <v>46520</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16" s="7">
         <v>26360</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="7">
         <v>6260</v>
       </c>
       <c r="M16">
@@ -1631,28 +2068,56 @@
       <c r="N16">
         <v>130840</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="12">
         <f t="shared" si="2"/>
         <v>0.19620903589236097</v>
       </c>
-      <c r="P16" s="16">
+      <c r="P16" s="12">
         <f t="shared" si="3"/>
         <v>0.69877821337494761</v>
       </c>
-      <c r="Q16" s="16">
+      <c r="Q16" s="12">
         <f t="shared" si="4"/>
         <v>0.50203631104175395</v>
       </c>
-      <c r="R16" s="16">
+      <c r="R16" s="12">
         <f t="shared" si="5"/>
         <v>0.10033113843108896</v>
       </c>
-      <c r="S16" s="16">
+      <c r="S16" s="12">
         <f t="shared" si="6"/>
         <v>2.382674228295208E-2</v>
       </c>
+      <c r="T16" s="12">
+        <f t="shared" si="7"/>
+        <v>0.50203631104175395</v>
+      </c>
+      <c r="U16" s="12">
+        <f t="shared" si="8"/>
+        <v>0.49800175084687703</v>
+      </c>
+      <c r="V16" s="12">
+        <f t="shared" si="9"/>
+        <v>17896.79213498675</v>
+      </c>
+      <c r="W16" s="12">
+        <f t="shared" si="10"/>
+        <v>2406.1522802273703</v>
+      </c>
+      <c r="X16" s="12">
+        <f t="shared" si="11"/>
+        <v>2757.7803432609089</v>
+      </c>
+      <c r="Y16" s="12">
+        <f t="shared" si="12"/>
+        <v>5256.4376427830384</v>
+      </c>
+      <c r="Z16" s="12">
+        <f t="shared" si="13"/>
+        <v>5163.9326234882792</v>
+      </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1660,7 +2125,7 @@
         <v>101290</v>
       </c>
       <c r="C17">
-        <v>8584699.8509999998</v>
+        <v>8.5846998509999999</v>
       </c>
       <c r="D17" s="2">
         <v>15596</v>
@@ -1678,16 +2143,16 @@
       <c r="H17">
         <v>29050</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="7">
         <v>77010</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="7">
         <v>7000</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="7">
         <v>14510</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="7">
         <v>2780</v>
       </c>
       <c r="M17">
@@ -1696,28 +2161,56 @@
       <c r="N17">
         <v>51260</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17" s="12">
         <f t="shared" si="2"/>
         <v>0.28680027643400136</v>
       </c>
-      <c r="P17" s="16">
+      <c r="P17" s="12">
         <f t="shared" si="3"/>
         <v>0.76029223023003256</v>
       </c>
-      <c r="Q17" s="16">
+      <c r="Q17" s="12">
         <f t="shared" si="4"/>
         <v>0.4940270510415638</v>
       </c>
-      <c r="R17" s="16">
+      <c r="R17" s="12">
         <f t="shared" si="5"/>
         <v>0.1432520485734031</v>
       </c>
-      <c r="S17" s="16">
+      <c r="S17" s="12">
         <f t="shared" si="6"/>
         <v>2.7445947280086879E-2</v>
       </c>
+      <c r="T17" s="12">
+        <f t="shared" si="7"/>
+        <v>0.4940270510415638</v>
+      </c>
+      <c r="U17" s="12">
+        <f t="shared" si="8"/>
+        <v>0.5060716753875012</v>
+      </c>
+      <c r="V17" s="12">
+        <f t="shared" si="9"/>
+        <v>11798.898244322556</v>
+      </c>
+      <c r="W17" s="12">
+        <f t="shared" si="10"/>
+        <v>1816.7204760435834</v>
+      </c>
+      <c r="X17" s="12">
+        <f t="shared" si="11"/>
+        <v>1957.5524236927688</v>
+      </c>
+      <c r="Y17" s="12">
+        <f t="shared" si="12"/>
+        <v>3757.4988712322311</v>
+      </c>
+      <c r="Z17" s="12">
+        <f t="shared" si="13"/>
+        <v>3774.272899736352</v>
+      </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1725,7 +2218,7 @@
         <v>46220</v>
       </c>
       <c r="C18">
-        <v>35044849.079999998</v>
+        <v>35.044849079999999</v>
       </c>
       <c r="D18" s="2">
         <v>4475</v>
@@ -1743,16 +2236,16 @@
       <c r="H18">
         <v>12190</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="7">
         <v>35050</v>
       </c>
-      <c r="J18" s="10">
+      <c r="J18" s="7">
         <v>3120</v>
       </c>
-      <c r="K18" s="10">
+      <c r="K18" s="7">
         <v>5510</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="7">
         <v>2530</v>
       </c>
       <c r="M18">
@@ -1761,28 +2254,56 @@
       <c r="N18">
         <v>24520</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18" s="12">
         <f t="shared" si="2"/>
         <v>0.2637386412808308</v>
       </c>
-      <c r="P18" s="16">
+      <c r="P18" s="12">
         <f t="shared" si="3"/>
         <v>0.75832972739073989</v>
       </c>
-      <c r="Q18" s="16">
+      <c r="Q18" s="12">
         <f t="shared" si="4"/>
         <v>0.46949372565988751</v>
       </c>
-      <c r="R18" s="16">
+      <c r="R18" s="12">
         <f t="shared" si="5"/>
         <v>0.11921246213760277</v>
       </c>
-      <c r="S18" s="16">
+      <c r="S18" s="12">
         <f t="shared" si="6"/>
         <v>5.4738208567719604E-2</v>
       </c>
+      <c r="T18" s="12">
+        <f t="shared" si="7"/>
+        <v>0.46949372565988751</v>
+      </c>
+      <c r="U18" s="12">
+        <f t="shared" si="8"/>
+        <v>0.53050627434011255</v>
+      </c>
+      <c r="V18" s="12">
+        <f t="shared" si="9"/>
+        <v>1318.8814109168936</v>
+      </c>
+      <c r="W18" s="12">
+        <f t="shared" si="10"/>
+        <v>127.69351609374944</v>
+      </c>
+      <c r="X18" s="12">
+        <f t="shared" si="11"/>
+        <v>258.04077453313431</v>
+      </c>
+      <c r="Y18" s="12">
+        <f t="shared" si="12"/>
+        <v>228.07916740499201</v>
+      </c>
+      <c r="Z18" s="12">
+        <f t="shared" si="13"/>
+        <v>385.73429062688376</v>
+      </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1790,7 +2311,7 @@
         <v>49330</v>
       </c>
       <c r="C19">
-        <v>8968011.8120000008</v>
+        <v>8.9680118120000003</v>
       </c>
       <c r="D19" s="2">
         <v>5420</v>
@@ -1808,16 +2329,16 @@
       <c r="H19">
         <v>11750</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="7">
         <v>40720</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="7">
         <v>1730</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="7">
         <v>4140</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="7">
         <v>2740</v>
       </c>
       <c r="M19">
@@ -1826,28 +2347,56 @@
       <c r="N19">
         <v>25400</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19" s="12">
         <f t="shared" si="2"/>
         <v>0.23819176971416989</v>
       </c>
-      <c r="P19" s="16">
+      <c r="P19" s="12">
         <f t="shared" si="3"/>
         <v>0.82546117980944655</v>
       </c>
-      <c r="Q19" s="16">
+      <c r="Q19" s="12">
         <f t="shared" si="4"/>
         <v>0.4851003446178796</v>
       </c>
-      <c r="R19" s="16">
+      <c r="R19" s="12">
         <f t="shared" si="5"/>
         <v>8.3924589499290492E-2</v>
       </c>
-      <c r="S19" s="16">
+      <c r="S19" s="12">
         <f t="shared" si="6"/>
         <v>5.5544293533346847E-2</v>
       </c>
+      <c r="T19" s="12">
+        <f t="shared" si="7"/>
+        <v>0.4851003446178796</v>
+      </c>
+      <c r="U19" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51489965538212046</v>
+      </c>
+      <c r="V19" s="12">
+        <f t="shared" si="9"/>
+        <v>5500.6618004218126</v>
+      </c>
+      <c r="W19" s="12">
+        <f t="shared" si="10"/>
+        <v>604.37030120182897</v>
+      </c>
+      <c r="X19" s="12">
+        <f t="shared" si="11"/>
+        <v>1116.7469679956305</v>
+      </c>
+      <c r="Y19" s="12">
+        <f t="shared" si="12"/>
+        <v>933.317236357806</v>
+      </c>
+      <c r="Z19" s="12">
+        <f t="shared" si="13"/>
+        <v>1721.1172691974593</v>
+      </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1855,7 +2404,7 @@
         <v>18340</v>
       </c>
       <c r="C20">
-        <v>1373186.2320000001</v>
+        <v>1.3731862320000001</v>
       </c>
       <c r="D20" s="2">
         <v>3167</v>
@@ -1873,16 +2422,16 @@
       <c r="H20">
         <v>6140</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="7">
         <v>14910</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="7">
         <v>1650</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="7">
         <v>1290</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="7">
         <v>480</v>
       </c>
       <c r="M20">
@@ -1891,28 +2440,56 @@
       <c r="N20">
         <v>9130</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="12">
         <f t="shared" si="2"/>
         <v>0.33478735005452565</v>
       </c>
-      <c r="P20" s="16">
+      <c r="P20" s="12">
         <f t="shared" si="3"/>
         <v>0.81297709923664119</v>
       </c>
-      <c r="Q20" s="16">
+      <c r="Q20" s="12">
         <f t="shared" si="4"/>
         <v>0.50218102508178841</v>
       </c>
-      <c r="R20" s="16">
+      <c r="R20" s="12">
         <f t="shared" si="5"/>
         <v>7.0338058887677204E-2</v>
       </c>
-      <c r="S20" s="16">
+      <c r="S20" s="12">
         <f t="shared" si="6"/>
         <v>2.6172300981461286E-2</v>
       </c>
+      <c r="T20" s="12">
+        <f t="shared" si="7"/>
+        <v>0.50218102508178841</v>
+      </c>
+      <c r="U20" s="12">
+        <f t="shared" si="8"/>
+        <v>0.49781897491821153</v>
+      </c>
+      <c r="V20" s="12">
+        <f t="shared" si="9"/>
+        <v>13355.799506734349</v>
+      </c>
+      <c r="W20" s="12">
+        <f t="shared" si="10"/>
+        <v>2306.3149966100154</v>
+      </c>
+      <c r="X20" s="12">
+        <f t="shared" si="11"/>
+        <v>1960.4041587856525</v>
+      </c>
+      <c r="Y20" s="12">
+        <f t="shared" si="12"/>
+        <v>5538.2145719037471</v>
+      </c>
+      <c r="Z20" s="12">
+        <f t="shared" si="13"/>
+        <v>4266.7191553956682</v>
+      </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1920,7 +2497,7 @@
         <v>147110</v>
       </c>
       <c r="C21">
-        <v>20489871.34</v>
+        <v>20.489871340000001</v>
       </c>
       <c r="D21" s="2">
         <v>13329</v>
@@ -1938,16 +2515,16 @@
       <c r="H21">
         <v>26570</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="7">
         <v>98790</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="7">
         <v>29370</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="7">
         <v>13120</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="7">
         <v>5840</v>
       </c>
       <c r="M21">
@@ -1956,28 +2533,56 @@
       <c r="N21">
         <v>74570</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="12">
         <f t="shared" si="2"/>
         <v>0.18061314662497452</v>
       </c>
-      <c r="P21" s="16">
+      <c r="P21" s="12">
         <f t="shared" si="3"/>
         <v>0.67153830466997488</v>
       </c>
-      <c r="Q21" s="16">
+      <c r="Q21" s="12">
         <f t="shared" si="4"/>
         <v>0.49310040106043096</v>
       </c>
-      <c r="R21" s="16">
+      <c r="R21" s="12">
         <f t="shared" si="5"/>
         <v>8.9184963632655836E-2</v>
       </c>
-      <c r="S21" s="16">
+      <c r="S21" s="12">
         <f t="shared" si="6"/>
         <v>3.9698185031608997E-2</v>
       </c>
+      <c r="T21" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49310040106043096</v>
+      </c>
+      <c r="U21" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50689959893956904</v>
+      </c>
+      <c r="V21" s="12">
+        <f t="shared" si="9"/>
+        <v>7179.6448869258738</v>
+      </c>
+      <c r="W21" s="12">
+        <f t="shared" si="10"/>
+        <v>650.51652979290986</v>
+      </c>
+      <c r="X21" s="12">
+        <f t="shared" si="11"/>
+        <v>1355.2061669509731</v>
+      </c>
+      <c r="Y21" s="12">
+        <f t="shared" si="12"/>
+        <v>1468.0424049944279</v>
+      </c>
+      <c r="Z21" s="12">
+        <f t="shared" si="13"/>
+        <v>2005.722696743883</v>
+      </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1985,7 +2590,7 @@
         <v>174450</v>
       </c>
       <c r="C22">
-        <v>12506232.73</v>
+        <v>12.506232730000001</v>
       </c>
       <c r="D22" s="2">
         <v>21102</v>
@@ -2003,16 +2608,16 @@
       <c r="H22">
         <v>19840</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="7">
         <v>131940</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="7">
         <v>26050</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="7">
         <v>12190</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="7">
         <v>4270</v>
       </c>
       <c r="M22">
@@ -2021,28 +2626,56 @@
       <c r="N22">
         <v>88520</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="12">
         <f t="shared" si="2"/>
         <v>0.11372886213814846</v>
       </c>
-      <c r="P22" s="16">
+      <c r="P22" s="12">
         <f t="shared" si="3"/>
         <v>0.75631986242476357</v>
       </c>
-      <c r="Q22" s="16">
+      <c r="Q22" s="12">
         <f t="shared" si="4"/>
         <v>0.49263399254800805</v>
       </c>
-      <c r="R22" s="16">
+      <c r="R22" s="12">
         <f t="shared" si="5"/>
         <v>6.9876755517340211E-2</v>
       </c>
-      <c r="S22" s="16">
+      <c r="S22" s="12">
         <f t="shared" si="6"/>
         <v>2.4476927486385785E-2</v>
       </c>
+      <c r="T22" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49263399254800805</v>
+      </c>
+      <c r="U22" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50742333046718258</v>
+      </c>
+      <c r="V22" s="12">
+        <f t="shared" si="9"/>
+        <v>13949.044749625413</v>
+      </c>
+      <c r="W22" s="12">
+        <f t="shared" si="10"/>
+        <v>1687.3186718635452</v>
+      </c>
+      <c r="X22" s="12">
+        <f t="shared" si="11"/>
+        <v>2521.3827921463921</v>
+      </c>
+      <c r="Y22" s="12">
+        <f t="shared" si="12"/>
+        <v>3920.844994542173</v>
+      </c>
+      <c r="Z22" s="12">
+        <f t="shared" si="13"/>
+        <v>4208.7014640099378</v>
+      </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -2050,7 +2683,7 @@
         <v>95930</v>
       </c>
       <c r="C23">
-        <v>35789538.979999997</v>
+        <v>35.789538979999996</v>
       </c>
       <c r="D23" s="2">
         <v>12670</v>
@@ -2068,16 +2701,16 @@
       <c r="H23">
         <v>26570</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="7">
         <v>78220</v>
       </c>
-      <c r="J23" s="10">
+      <c r="J23" s="7">
         <v>6940</v>
       </c>
-      <c r="K23" s="10">
+      <c r="K23" s="7">
         <v>7060</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="7">
         <v>3710</v>
       </c>
       <c r="M23">
@@ -2086,28 +2719,56 @@
       <c r="N23">
         <v>50820</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23" s="12">
         <f t="shared" si="2"/>
         <v>0.27697279266131553</v>
       </c>
-      <c r="P23" s="16">
+      <c r="P23" s="12">
         <f t="shared" si="3"/>
         <v>0.81538621911810694</v>
       </c>
-      <c r="Q23" s="16">
+      <c r="Q23" s="12">
         <f t="shared" si="4"/>
         <v>0.47034295840717188</v>
       </c>
-      <c r="R23" s="16">
+      <c r="R23" s="12">
         <f t="shared" si="5"/>
         <v>7.359532992807255E-2</v>
       </c>
-      <c r="S23" s="16">
+      <c r="S23" s="12">
         <f t="shared" si="6"/>
         <v>3.8674033149171269E-2</v>
       </c>
+      <c r="T23" s="12">
+        <f t="shared" si="7"/>
+        <v>0.47034295840717188</v>
+      </c>
+      <c r="U23" s="12">
+        <f t="shared" si="8"/>
+        <v>0.52976128426978009</v>
+      </c>
+      <c r="V23" s="12">
+        <f t="shared" si="9"/>
+        <v>2680.3921686056883</v>
+      </c>
+      <c r="W23" s="12">
+        <f t="shared" si="10"/>
+        <v>354.01406000452488</v>
+      </c>
+      <c r="X23" s="12">
+        <f t="shared" si="11"/>
+        <v>464.04621219851214</v>
+      </c>
+      <c r="Y23" s="12">
+        <f t="shared" si="12"/>
+        <v>873.41164180595445</v>
+      </c>
+      <c r="Z23" s="12">
+        <f t="shared" si="13"/>
+        <v>818.06027220303702</v>
+      </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -2115,7 +2776,7 @@
         <v>10070</v>
       </c>
       <c r="C24">
-        <v>1475697.9650000001</v>
+        <v>1.4756979650000002</v>
       </c>
       <c r="D24" s="2">
         <v>600</v>
@@ -2133,16 +2794,16 @@
       <c r="H24">
         <v>1900</v>
       </c>
-      <c r="I24" s="10">
+      <c r="I24" s="7">
         <v>7020</v>
       </c>
-      <c r="J24" s="10">
+      <c r="J24" s="7">
         <v>90</v>
       </c>
-      <c r="K24" s="10">
+      <c r="K24" s="7">
         <v>1500</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="7">
         <v>1460</v>
       </c>
       <c r="M24">
@@ -2151,28 +2812,56 @@
       <c r="N24">
         <v>5450</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24" s="12">
         <f t="shared" si="2"/>
         <v>0.18867924528301888</v>
       </c>
-      <c r="P24" s="16">
+      <c r="P24" s="12">
         <f t="shared" si="3"/>
         <v>0.69712015888778545</v>
       </c>
-      <c r="Q24" s="16">
+      <c r="Q24" s="12">
         <f t="shared" si="4"/>
         <v>0.45878848063555117</v>
       </c>
-      <c r="R24" s="16">
+      <c r="R24" s="12">
         <f t="shared" si="5"/>
         <v>0.14895729890764647</v>
       </c>
-      <c r="S24" s="16">
+      <c r="S24" s="12">
         <f t="shared" si="6"/>
         <v>0.14498510427010924</v>
       </c>
+      <c r="T24" s="12">
+        <f t="shared" si="7"/>
+        <v>0.45878848063555117</v>
+      </c>
+      <c r="U24" s="12">
+        <f t="shared" si="8"/>
+        <v>0.54121151936444889</v>
+      </c>
+      <c r="V24" s="12">
+        <f t="shared" si="9"/>
+        <v>6823.889602639656</v>
+      </c>
+      <c r="W24" s="12">
+        <f t="shared" si="10"/>
+        <v>406.58726530127046</v>
+      </c>
+      <c r="X24" s="12">
+        <f t="shared" si="11"/>
+        <v>1899.4401743991018</v>
+      </c>
+      <c r="Y24" s="12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Z24" s="12">
+        <f t="shared" si="13"/>
+        <v>2306.0274397003723</v>
+      </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -2180,7 +2869,7 @@
         <v>102640</v>
       </c>
       <c r="C25">
-        <v>18058884.27</v>
+        <v>18.05888427</v>
       </c>
       <c r="D25" s="2">
         <v>13667</v>
@@ -2198,16 +2887,16 @@
       <c r="H25">
         <v>14700</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="7">
         <v>72910</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="7">
         <v>16680</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="7">
         <v>9360</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="7">
         <v>3680</v>
       </c>
       <c r="M25">
@@ -2216,28 +2905,56 @@
       <c r="N25">
         <v>51930</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25" s="12">
         <f t="shared" si="2"/>
         <v>0.14321901792673422</v>
       </c>
-      <c r="P25" s="16">
+      <c r="P25" s="12">
         <f t="shared" si="3"/>
         <v>0.71034684333593145</v>
       </c>
-      <c r="Q25" s="16">
+      <c r="Q25" s="12">
         <f t="shared" si="4"/>
         <v>0.49405689789555729</v>
       </c>
-      <c r="R25" s="16">
+      <c r="R25" s="12">
         <f t="shared" si="5"/>
         <v>9.1192517537022608E-2</v>
       </c>
-      <c r="S25" s="16">
+      <c r="S25" s="12">
         <f t="shared" si="6"/>
         <v>3.5853468433359313E-2</v>
       </c>
+      <c r="T25" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49405689789555729</v>
+      </c>
+      <c r="U25" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50594310210444271</v>
+      </c>
+      <c r="V25" s="12">
+        <f t="shared" si="9"/>
+        <v>5683.6290916659163</v>
+      </c>
+      <c r="W25" s="12">
+        <f t="shared" si="10"/>
+        <v>756.80201476810282</v>
+      </c>
+      <c r="X25" s="12">
+        <f t="shared" si="11"/>
+        <v>922.98060892329977</v>
+      </c>
+      <c r="Y25" s="12">
+        <f t="shared" si="12"/>
+        <v>1582.8220377647949</v>
+      </c>
+      <c r="Z25" s="12">
+        <f t="shared" si="13"/>
+        <v>1679.7826236914027</v>
+      </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -2245,7 +2962,7 @@
         <v>249370</v>
       </c>
       <c r="C26">
-        <v>10603045.039999999</v>
+        <v>10.60304504</v>
       </c>
       <c r="D26" s="2">
         <v>29774</v>
@@ -2263,16 +2980,16 @@
       <c r="H26">
         <v>37870</v>
       </c>
-      <c r="I26" s="10">
+      <c r="I26" s="7">
         <v>192870</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="7">
         <v>28560</v>
       </c>
-      <c r="K26" s="10">
+      <c r="K26" s="7">
         <v>21690</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="7">
         <v>6240</v>
       </c>
       <c r="M26">
@@ -2281,28 +2998,56 @@
       <c r="N26">
         <v>126890</v>
       </c>
-      <c r="O26" s="16">
+      <c r="O26" s="12">
         <f t="shared" si="2"/>
         <v>0.15186269398885191</v>
       </c>
-      <c r="P26" s="16">
+      <c r="P26" s="12">
         <f t="shared" si="3"/>
         <v>0.77342904118378308</v>
       </c>
-      <c r="Q26" s="16">
+      <c r="Q26" s="12">
         <f t="shared" si="4"/>
         <v>0.49115771744796888</v>
       </c>
-      <c r="R26" s="16">
+      <c r="R26" s="12">
         <f t="shared" si="5"/>
         <v>8.6979187552632634E-2</v>
       </c>
-      <c r="S26" s="16">
+      <c r="S26" s="12">
         <f t="shared" si="6"/>
         <v>2.50230581064282E-2</v>
       </c>
+      <c r="T26" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49115771744796888</v>
+      </c>
+      <c r="U26" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50884228255203112</v>
+      </c>
+      <c r="V26" s="12">
+        <f t="shared" si="9"/>
+        <v>23518.715525516622</v>
+      </c>
+      <c r="W26" s="12">
+        <f t="shared" si="10"/>
+        <v>2808.0612585985959</v>
+      </c>
+      <c r="X26" s="12">
+        <f t="shared" si="11"/>
+        <v>4147.8650551879582</v>
+      </c>
+      <c r="Y26" s="12">
+        <f t="shared" si="12"/>
+        <v>6430.2282733677803</v>
+      </c>
+      <c r="Z26" s="12">
+        <f t="shared" si="13"/>
+        <v>6955.9263137865537</v>
+      </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -2310,7 +3055,7 @@
         <v>116900</v>
       </c>
       <c r="C27">
-        <v>10100540.689999999</v>
+        <v>10.100540689999999</v>
       </c>
       <c r="D27" s="2">
         <v>11615</v>
@@ -2328,16 +3073,16 @@
       <c r="H27">
         <v>32590</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="7">
         <v>98770</v>
       </c>
-      <c r="J27" s="10">
+      <c r="J27" s="7">
         <v>4860</v>
       </c>
-      <c r="K27" s="10">
+      <c r="K27" s="7">
         <v>10250</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="7">
         <v>3020</v>
       </c>
       <c r="M27">
@@ -2346,28 +3091,56 @@
       <c r="N27">
         <v>60530</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27" s="12">
         <f t="shared" si="2"/>
         <v>0.27878528656971768</v>
       </c>
-      <c r="P27" s="16">
+      <c r="P27" s="12">
         <f t="shared" si="3"/>
         <v>0.84491017964071857</v>
       </c>
-      <c r="Q27" s="16">
+      <c r="Q27" s="12">
         <f t="shared" si="4"/>
         <v>0.48220701454234388</v>
       </c>
-      <c r="R27" s="16">
+      <c r="R27" s="12">
         <f t="shared" si="5"/>
         <v>8.7681779298545759E-2</v>
       </c>
-      <c r="S27" s="16">
+      <c r="S27" s="12">
         <f t="shared" si="6"/>
         <v>2.5834046193327631E-2</v>
       </c>
+      <c r="T27" s="12">
+        <f t="shared" si="7"/>
+        <v>0.48220701454234388</v>
+      </c>
+      <c r="U27" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51779298545765606</v>
+      </c>
+      <c r="V27" s="12">
+        <f t="shared" si="9"/>
+        <v>11573.637846510177</v>
+      </c>
+      <c r="W27" s="12">
+        <f t="shared" si="10"/>
+        <v>1149.9384395826835</v>
+      </c>
+      <c r="X27" s="12">
+        <f t="shared" si="11"/>
+        <v>2094.2443230729664</v>
+      </c>
+      <c r="Y27" s="12">
+        <f t="shared" si="12"/>
+        <v>2186.516611122132</v>
+      </c>
+      <c r="Z27" s="12">
+        <f t="shared" si="13"/>
+        <v>3244.1827626556496</v>
+      </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -2375,7 +3148,7 @@
         <v>259900</v>
       </c>
       <c r="C28">
-        <v>30676070.77</v>
+        <v>30.676070769999999</v>
       </c>
       <c r="D28" s="2">
         <v>32006</v>
@@ -2393,16 +3166,16 @@
       <c r="H28">
         <v>59620</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="7">
         <v>173660</v>
       </c>
-      <c r="J28" s="10">
+      <c r="J28" s="7">
         <v>56570</v>
       </c>
-      <c r="K28" s="10">
+      <c r="K28" s="7">
         <v>21700</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="7">
         <v>7970</v>
       </c>
       <c r="M28">
@@ -2411,28 +3184,56 @@
       <c r="N28">
         <v>132900</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28" s="12">
         <f t="shared" si="2"/>
         <v>0.2293959215082724</v>
       </c>
-      <c r="P28" s="16">
+      <c r="P28" s="12">
         <f t="shared" si="3"/>
         <v>0.66818006925740669</v>
       </c>
-      <c r="Q28" s="16">
+      <c r="Q28" s="12">
         <f t="shared" si="4"/>
         <v>0.48864948056944979</v>
       </c>
-      <c r="R28" s="16">
+      <c r="R28" s="12">
         <f t="shared" si="5"/>
         <v>8.3493651404386304E-2</v>
       </c>
-      <c r="S28" s="16">
+      <c r="S28" s="12">
         <f t="shared" si="6"/>
         <v>3.0665640631011928E-2</v>
       </c>
+      <c r="T28" s="12">
+        <f t="shared" si="7"/>
+        <v>0.48864948056944979</v>
+      </c>
+      <c r="U28" s="12">
+        <f t="shared" si="8"/>
+        <v>0.51135051943055021</v>
+      </c>
+      <c r="V28" s="12">
+        <f t="shared" si="9"/>
+        <v>8472.4018909935512</v>
+      </c>
+      <c r="W28" s="12">
+        <f t="shared" si="10"/>
+        <v>1043.3539627669859</v>
+      </c>
+      <c r="X28" s="12">
+        <f t="shared" si="11"/>
+        <v>1370.6123028350285</v>
+      </c>
+      <c r="Y28" s="12">
+        <f t="shared" si="12"/>
+        <v>2374.6848332101431</v>
+      </c>
+      <c r="Z28" s="12">
+        <f t="shared" si="13"/>
+        <v>2413.9662656020141</v>
+      </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -2440,7 +3241,7 @@
         <v>21810</v>
       </c>
       <c r="C29">
-        <v>7552299.2810000004</v>
+        <v>7.5522992810000007</v>
       </c>
       <c r="D29" s="2">
         <v>973</v>
@@ -2458,16 +3259,16 @@
       <c r="H29">
         <v>4460</v>
       </c>
-      <c r="I29" s="10">
+      <c r="I29" s="7">
         <v>16270</v>
       </c>
-      <c r="J29" s="10">
+      <c r="J29" s="7">
         <v>240</v>
       </c>
-      <c r="K29" s="10">
+      <c r="K29" s="7">
         <v>2200</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="7">
         <v>3090</v>
       </c>
       <c r="M29">
@@ -2476,28 +3277,56 @@
       <c r="N29">
         <v>11700</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29" s="12">
         <f t="shared" si="2"/>
         <v>0.20449335167354424</v>
       </c>
-      <c r="P29" s="16">
+      <c r="P29" s="12">
         <f t="shared" si="3"/>
         <v>0.74598807886290697</v>
       </c>
-      <c r="Q29" s="16">
+      <c r="Q29" s="12">
         <f t="shared" si="4"/>
         <v>0.46309032553874369</v>
       </c>
-      <c r="R29" s="16">
+      <c r="R29" s="12">
         <f t="shared" si="5"/>
         <v>0.10087116001834021</v>
       </c>
-      <c r="S29" s="16">
+      <c r="S29" s="12">
         <f t="shared" si="6"/>
         <v>0.14167812929848694</v>
       </c>
+      <c r="T29" s="12">
+        <f t="shared" si="7"/>
+        <v>0.46309032553874369</v>
+      </c>
+      <c r="U29" s="12">
+        <f t="shared" si="8"/>
+        <v>0.53645116918844571</v>
+      </c>
+      <c r="V29" s="12">
+        <f t="shared" si="9"/>
+        <v>2887.8622507544665</v>
+      </c>
+      <c r="W29" s="12">
+        <f t="shared" si="10"/>
+        <v>128.83493672554314</v>
+      </c>
+      <c r="X29" s="12">
+        <f t="shared" si="11"/>
+        <v>761.88717977263639</v>
+      </c>
+      <c r="Y29" s="12">
+        <f t="shared" si="12"/>
+        <v>24.76067129257612</v>
+      </c>
+      <c r="Z29" s="12">
+        <f t="shared" si="13"/>
+        <v>890.7221164981795</v>
+      </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -2505,7 +3334,7 @@
         <v>121850</v>
       </c>
       <c r="C30">
-        <v>8180210.3660000004</v>
+        <v>8.1802103660000007</v>
       </c>
       <c r="D30" s="2">
         <v>17718</v>
@@ -2523,16 +3352,16 @@
       <c r="H30">
         <v>34950</v>
       </c>
-      <c r="I30" s="10">
+      <c r="I30" s="7">
         <v>101320</v>
       </c>
-      <c r="J30" s="10">
+      <c r="J30" s="7">
         <v>8410</v>
       </c>
-      <c r="K30" s="10">
+      <c r="K30" s="7">
         <v>8590</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="7">
         <v>3530</v>
       </c>
       <c r="M30">
@@ -2541,28 +3370,56 @@
       <c r="N30">
         <v>63960</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30" s="12">
         <f t="shared" si="2"/>
         <v>0.28682806729585558</v>
       </c>
-      <c r="P30" s="16">
+      <c r="P30" s="12">
         <f t="shared" si="3"/>
         <v>0.83151415675010254</v>
       </c>
-      <c r="Q30" s="16">
+      <c r="Q30" s="12">
         <f t="shared" si="4"/>
         <v>0.47509232663110379</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30" s="12">
         <f t="shared" si="5"/>
         <v>7.049651210504719E-2</v>
       </c>
-      <c r="S30" s="16">
+      <c r="S30" s="12">
         <f t="shared" si="6"/>
         <v>2.8970045137464095E-2</v>
       </c>
+      <c r="T30" s="12">
+        <f t="shared" si="7"/>
+        <v>0.47509232663110379</v>
+      </c>
+      <c r="U30" s="12">
+        <f t="shared" si="8"/>
+        <v>0.52490767336889621</v>
+      </c>
+      <c r="V30" s="12">
+        <f t="shared" si="9"/>
+        <v>14895.704945004099</v>
+      </c>
+      <c r="W30" s="12">
+        <f t="shared" si="10"/>
+        <v>2165.9589677109775</v>
+      </c>
+      <c r="X30" s="12">
+        <f t="shared" si="11"/>
+        <v>2340.6488517192734</v>
+      </c>
+      <c r="Y30" s="12">
+        <f t="shared" si="12"/>
+        <v>4800.854530982363</v>
+      </c>
+      <c r="Z30" s="12">
+        <f t="shared" si="13"/>
+        <v>4506.6078194302509</v>
+      </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -2570,7 +3427,7 @@
         <v>255130</v>
       </c>
       <c r="C31">
-        <v>15619408.300000001</v>
+        <v>15.6194083</v>
       </c>
       <c r="D31" s="2">
         <v>35716</v>
@@ -2588,16 +3445,16 @@
       <c r="H31">
         <v>41480</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="7">
         <v>155360</v>
       </c>
-      <c r="J31" s="10">
+      <c r="J31" s="7">
         <v>65480</v>
       </c>
-      <c r="K31" s="10">
+      <c r="K31" s="7">
         <v>28240</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="7">
         <v>6060</v>
       </c>
       <c r="M31">
@@ -2606,28 +3463,56 @@
       <c r="N31">
         <v>127150</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31" s="12">
         <f t="shared" si="2"/>
         <v>0.1625837808176224</v>
       </c>
-      <c r="P31" s="16">
+      <c r="P31" s="12">
         <f t="shared" si="3"/>
         <v>0.60894445968721833</v>
       </c>
-      <c r="Q31" s="16">
+      <c r="Q31" s="12">
         <f t="shared" si="4"/>
         <v>0.50166581742641003</v>
       </c>
-      <c r="R31" s="16">
+      <c r="R31" s="12">
         <f t="shared" si="5"/>
         <v>0.11068866852193</v>
       </c>
-      <c r="S31" s="16">
+      <c r="S31" s="12">
         <f t="shared" si="6"/>
         <v>2.3752596715399994E-2</v>
       </c>
+      <c r="T31" s="12">
+        <f t="shared" si="7"/>
+        <v>0.50166581742641003</v>
+      </c>
+      <c r="U31" s="12">
+        <f t="shared" si="8"/>
+        <v>0.49837337827774075</v>
+      </c>
+      <c r="V31" s="12">
+        <f t="shared" si="9"/>
+        <v>16334.165488202265</v>
+      </c>
+      <c r="W31" s="12">
+        <f t="shared" si="10"/>
+        <v>2286.6423179423514</v>
+      </c>
+      <c r="X31" s="12">
+        <f t="shared" si="11"/>
+        <v>2304.3766645116766</v>
+      </c>
+      <c r="Y31" s="12">
+        <f t="shared" si="12"/>
+        <v>4671.4317596781175</v>
+      </c>
+      <c r="Z31" s="12">
+        <f t="shared" si="13"/>
+        <v>4591.0189824540284</v>
+      </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -2635,7 +3520,7 @@
         <v>221610</v>
       </c>
       <c r="C32">
-        <v>21011029.079999998</v>
+        <v>21.011029079999997</v>
       </c>
       <c r="D32" s="2">
         <v>34738</v>
@@ -2653,16 +3538,16 @@
       <c r="H32">
         <v>44690</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="7">
         <v>153160</v>
       </c>
-      <c r="J32" s="10">
+      <c r="J32" s="7">
         <v>40390</v>
       </c>
-      <c r="K32" s="10">
+      <c r="K32" s="7">
         <v>21950</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="7">
         <v>6110</v>
       </c>
       <c r="M32">
@@ -2671,28 +3556,57 @@
       <c r="N32">
         <v>112140</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32" s="12">
         <f t="shared" si="2"/>
         <v>0.20166057488380487</v>
       </c>
-      <c r="P32" s="16">
+      <c r="P32" s="12">
         <f t="shared" si="3"/>
         <v>0.69112404674879291</v>
       </c>
-      <c r="Q32" s="16">
+      <c r="Q32" s="12">
         <f t="shared" si="4"/>
         <v>0.49397590361445781</v>
       </c>
-      <c r="R32" s="16">
+      <c r="R32" s="12">
         <f t="shared" si="5"/>
         <v>9.9047876900861878E-2</v>
       </c>
-      <c r="S32" s="16">
+      <c r="S32" s="12">
         <f t="shared" si="6"/>
         <v>2.7570957989260413E-2</v>
+      </c>
+      <c r="T32" s="12">
+        <f t="shared" si="7"/>
+        <v>0.49397590361445781</v>
+      </c>
+      <c r="U32" s="12">
+        <f t="shared" si="8"/>
+        <v>0.50602409638554213</v>
+      </c>
+      <c r="V32" s="12">
+        <f t="shared" si="9"/>
+        <v>10547.317751844263</v>
+      </c>
+      <c r="W32" s="12">
+        <f t="shared" si="10"/>
+        <v>1653.3221608391589</v>
+      </c>
+      <c r="X32" s="12">
+        <f t="shared" si="11"/>
+        <v>1521.3914500945523</v>
+      </c>
+      <c r="Y32" s="12">
+        <f t="shared" si="12"/>
+        <v>3177.9976004868777</v>
+      </c>
+      <c r="Z32" s="12">
+        <f t="shared" si="13"/>
+        <v>3174.7136109337112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>